<commit_message>
TMA Harvest Receipt report changes
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="662">
   <si>
     <t>Abilene</t>
   </si>
@@ -1388,9 +1388,6 @@
     <t>CANTON TERM BUNKER</t>
   </si>
   <si>
-    <t>SOUTH</t>
-  </si>
-  <si>
     <t>CANTON TERMINAL</t>
   </si>
   <si>
@@ -1724,9 +1721,6 @@
     <t>HILLSBORO</t>
   </si>
   <si>
-    <t>EAST</t>
-  </si>
-  <si>
     <t>ALTA VISTA BUNKER</t>
   </si>
   <si>
@@ -1790,9 +1784,6 @@
     <t>DIRECT - WALTON</t>
   </si>
   <si>
-    <t>NORTH</t>
-  </si>
-  <si>
     <t>BENNINGTON BUNKER</t>
   </si>
   <si>
@@ -2015,7 +2006,13 @@
     <t>HUTCH COMMERICAL ELV</t>
   </si>
   <si>
-    <t>FarCoop</t>
+    <t>MKC</t>
+  </si>
+  <si>
+    <t>Far Coop</t>
+  </si>
+  <si>
+    <t>CPC</t>
   </si>
 </sst>
 </file>
@@ -6558,37 +6555,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="F1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="G1" t="s">
         <v>73</v>
       </c>
       <c r="H1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="I1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="J1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="K1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="L1" t="s">
         <v>244</v>
@@ -6605,25 +6602,25 @@
         <v>274</v>
       </c>
       <c r="D2" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E2">
-        <v>1478000</v>
+        <v>1330200</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>84</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6631,10 +6628,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>645</v>
-      </c>
-      <c r="D3" t="s">
-        <v>453</v>
+        <v>642</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -6650,22 +6644,22 @@
         <v>251</v>
       </c>
       <c r="D4" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E4">
-        <v>790000</v>
+        <v>651600</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>101</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6676,25 +6670,25 @@
         <v>258</v>
       </c>
       <c r="D5" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E5">
-        <v>3460000</v>
+        <v>3120000</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>135</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6702,10 +6696,13 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D6" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E6">
+        <v>1000000</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -6720,14 +6717,11 @@
       <c r="B7" t="s">
         <v>273</v>
       </c>
-      <c r="D7" t="s">
-        <v>662</v>
-      </c>
       <c r="F7" s="4" t="s">
         <v>121</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>162</v>
@@ -6741,25 +6735,25 @@
         <v>260</v>
       </c>
       <c r="D8" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E8">
-        <v>1467000</v>
+        <v>1318300</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -6770,28 +6764,28 @@
         <v>382</v>
       </c>
       <c r="D9" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E9">
-        <v>1109000</v>
+        <v>1053900</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>137</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -6802,16 +6796,16 @@
         <v>257</v>
       </c>
       <c r="D10" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E10">
-        <v>205000</v>
+        <v>184500</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>131</v>
@@ -6825,22 +6819,22 @@
         <v>256</v>
       </c>
       <c r="D11" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E11">
-        <v>643000</v>
+        <v>607500</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>128</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -6848,22 +6842,22 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D12" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E12">
-        <v>288000</v>
+        <v>259200</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -6874,22 +6868,22 @@
         <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E13">
-        <v>499000</v>
+        <v>406200</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>112</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -6900,19 +6894,22 @@
         <v>335</v>
       </c>
       <c r="D14" t="s">
-        <v>662</v>
+        <v>659</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>284</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -6923,22 +6920,25 @@
         <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>453</v>
+        <v>659</v>
+      </c>
+      <c r="E15">
+        <v>232200</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>122</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6946,16 +6946,19 @@
         <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D16" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E16">
+        <v>165655</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>124</v>
@@ -6966,19 +6969,19 @@
         <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D17" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E17">
-        <v>279000</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>186</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>188</v>
@@ -6995,13 +6998,16 @@
         <v>428</v>
       </c>
       <c r="D18" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E18">
+        <v>421000</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>208</v>
@@ -7015,10 +7021,10 @@
         <v>358</v>
       </c>
       <c r="D19" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E19">
-        <v>577000</v>
+        <v>519300</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>2</v>
@@ -7030,7 +7036,7 @@
         <v>92</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7038,10 +7044,13 @@
         <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D20" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E20">
+        <v>235800</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -7055,10 +7064,13 @@
         <v>182</v>
       </c>
       <c r="B21" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D21" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E21">
+        <v>354600</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -7070,13 +7082,13 @@
         <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D22" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E22">
-        <v>391000</v>
+        <v>352000</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>18</v>
@@ -7096,10 +7108,13 @@
         <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D23" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E23">
+        <v>765000</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -7110,19 +7125,19 @@
         <v>187</v>
       </c>
       <c r="B24" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D24" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E24">
-        <v>2099000</v>
+        <v>900000</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>184</v>
@@ -7133,10 +7148,13 @@
         <v>188</v>
       </c>
       <c r="B25" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D25" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E25">
+        <v>1000000</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -7147,10 +7165,13 @@
         <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D26" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E26">
+        <v>800000</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -7165,22 +7186,22 @@
         <v>262</v>
       </c>
       <c r="D27" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E27">
-        <v>1615000</v>
+        <v>485500</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>156</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7191,25 +7212,25 @@
         <v>267</v>
       </c>
       <c r="D28" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E28">
-        <v>1266000</v>
+        <v>1060000</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>194</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -7220,22 +7241,22 @@
         <v>261</v>
       </c>
       <c r="D29" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E29">
-        <v>260000</v>
+        <v>234000</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>149</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -7246,22 +7267,22 @@
         <v>266</v>
       </c>
       <c r="D30" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E30">
-        <v>758000</v>
+        <v>509000</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>192</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -7272,22 +7293,22 @@
         <v>247</v>
       </c>
       <c r="D31" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E31">
-        <v>716000</v>
+        <v>644000</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>87</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -7298,10 +7319,10 @@
         <v>249</v>
       </c>
       <c r="D32" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E32">
-        <v>521000</v>
+        <v>182000</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>3</v>
@@ -7313,7 +7334,7 @@
         <v>94</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -7321,10 +7342,13 @@
         <v>197</v>
       </c>
       <c r="B33" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D33" t="s">
-        <v>662</v>
+        <v>659</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -7339,10 +7363,10 @@
         <v>372</v>
       </c>
       <c r="D34" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="E34">
-        <v>357000</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>114</v>
@@ -7359,10 +7383,13 @@
         <v>199</v>
       </c>
       <c r="B35" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D35" t="s">
-        <v>587</v>
+        <v>659</v>
+      </c>
+      <c r="E35">
+        <v>319000</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -7374,10 +7401,7 @@
         <v>201</v>
       </c>
       <c r="B36" t="s">
-        <v>586</v>
-      </c>
-      <c r="D36" t="s">
-        <v>662</v>
+        <v>584</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -7391,10 +7415,10 @@
         <v>425</v>
       </c>
       <c r="D37" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E37">
-        <v>1985000</v>
+        <v>1620000</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>203</v>
@@ -7414,10 +7438,10 @@
         <v>268</v>
       </c>
       <c r="D38" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E38">
-        <v>1318000</v>
+        <v>1186200</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>32</v>
@@ -7429,10 +7453,10 @@
         <v>196</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -7440,13 +7464,13 @@
         <v>215</v>
       </c>
       <c r="B39" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D39" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E39">
-        <v>1944000</v>
+        <v>2000000</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -7462,22 +7486,22 @@
         <v>264</v>
       </c>
       <c r="D40" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E40">
-        <v>801000</v>
+        <v>683000</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>180</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -7488,22 +7512,22 @@
         <v>252</v>
       </c>
       <c r="D41" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E41">
-        <v>1262000</v>
+        <v>1100000</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>105</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -7511,13 +7535,13 @@
         <v>245</v>
       </c>
       <c r="B42" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D42" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E42">
-        <v>427000</v>
+        <v>375000</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -7532,16 +7556,16 @@
         <v>255</v>
       </c>
       <c r="D43" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E43">
-        <v>262000</v>
+        <v>235800</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>126</v>
@@ -7555,25 +7579,25 @@
         <v>262</v>
       </c>
       <c r="B44" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D44" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E44">
-        <v>436000</v>
+        <v>388800</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>176</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -7584,22 +7608,22 @@
         <v>269</v>
       </c>
       <c r="D45" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E45">
-        <v>1113000</v>
+        <v>961600</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>202</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -7610,7 +7634,10 @@
         <v>440</v>
       </c>
       <c r="D46" t="s">
-        <v>662</v>
+        <v>659</v>
+      </c>
+      <c r="E46">
+        <v>84600</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -7622,10 +7649,13 @@
         <v>291</v>
       </c>
       <c r="B47" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D47" t="s">
-        <v>453</v>
+        <v>659</v>
+      </c>
+      <c r="E47">
+        <v>540000</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -7640,22 +7670,22 @@
         <v>250</v>
       </c>
       <c r="D48" t="s">
-        <v>453</v>
+        <v>659</v>
       </c>
       <c r="E48">
-        <v>1114000</v>
+        <v>837000</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>98</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -7666,10 +7696,10 @@
         <v>272</v>
       </c>
       <c r="D49" t="s">
-        <v>565</v>
+        <v>659</v>
       </c>
       <c r="E49">
-        <v>1266000</v>
+        <v>1140000</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>23</v>
@@ -7689,16 +7719,16 @@
         <v>248</v>
       </c>
       <c r="D50" t="s">
-        <v>565</v>
+        <v>659</v>
       </c>
       <c r="E50">
-        <v>747000</v>
+        <v>675000</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>90</v>
@@ -7712,16 +7742,16 @@
         <v>263</v>
       </c>
       <c r="D51" t="s">
-        <v>565</v>
+        <v>659</v>
       </c>
       <c r="E51">
-        <v>1106000</v>
+        <v>1267000</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>178</v>
@@ -7732,13 +7762,13 @@
         <v>296</v>
       </c>
       <c r="B52" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D52" t="s">
-        <v>565</v>
+        <v>659</v>
       </c>
       <c r="E52">
-        <v>469000</v>
+        <v>400000</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -7749,28 +7779,31 @@
         <v>311</v>
       </c>
       <c r="B53" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D53" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E53">
+        <v>1328500</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -7778,10 +7811,13 @@
         <v>315</v>
       </c>
       <c r="B54" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D54" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E54">
+        <v>400000</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -7795,22 +7831,25 @@
         <v>331</v>
       </c>
       <c r="B55" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D55" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E55">
+        <v>218560</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -7818,22 +7857,25 @@
         <v>341</v>
       </c>
       <c r="B56" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D56" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E56">
+        <v>993000</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -7844,19 +7886,22 @@
         <v>367</v>
       </c>
       <c r="D57" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E57">
+        <v>550800</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -7864,16 +7909,19 @@
         <v>361</v>
       </c>
       <c r="B58" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D58" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E58">
+        <v>345600</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K58" s="4"/>
     </row>
@@ -7882,10 +7930,13 @@
         <v>432</v>
       </c>
       <c r="B59" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D59" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E59">
+        <v>2255500</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -7896,22 +7947,25 @@
         <v>433</v>
       </c>
       <c r="B60" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D60" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E60">
+        <v>2255500</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -7919,22 +7973,25 @@
         <v>442</v>
       </c>
       <c r="B61" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D61" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E61">
+        <v>867600</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -7942,22 +7999,25 @@
         <v>443</v>
       </c>
       <c r="B62" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D62" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E62">
+        <v>1293000</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -7965,10 +8025,13 @@
         <v>445</v>
       </c>
       <c r="B63" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D63" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E63">
+        <v>500000</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -7980,19 +8043,22 @@
         <v>447</v>
       </c>
       <c r="B64" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D64" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="E64">
+        <v>900000</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -8000,22 +8066,25 @@
         <v>510</v>
       </c>
       <c r="B65" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D65" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E65">
+        <v>1175000</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -8026,19 +8095,22 @@
         <v>369</v>
       </c>
       <c r="D66" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E66">
+        <v>233100</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>111</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -8046,22 +8118,25 @@
         <v>530</v>
       </c>
       <c r="B67" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D67" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E67">
+        <v>326700</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -8069,22 +8144,25 @@
         <v>540</v>
       </c>
       <c r="B68" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D68" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E68">
+        <v>376200</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -8092,19 +8170,22 @@
         <v>541</v>
       </c>
       <c r="B69" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D69" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E69">
+        <v>1053000</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -8112,22 +8193,25 @@
         <v>542</v>
       </c>
       <c r="B70" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D70" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E70">
+        <v>1040400</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -8135,22 +8219,25 @@
         <v>543</v>
       </c>
       <c r="B71" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D71" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E71">
+        <v>1356000</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -8158,22 +8245,25 @@
         <v>544</v>
       </c>
       <c r="B72" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D72" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E72">
+        <v>839000</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -8181,19 +8271,22 @@
         <v>545</v>
       </c>
       <c r="B73" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D73" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E73">
+        <v>529000</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -8201,22 +8294,25 @@
         <v>546</v>
       </c>
       <c r="B74" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D74" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E74">
+        <v>428000</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -8224,22 +8320,25 @@
         <v>547</v>
       </c>
       <c r="B75" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D75" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E75">
+        <v>561000</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -8247,22 +8346,25 @@
         <v>548</v>
       </c>
       <c r="B76" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D76" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E76">
+        <v>460000</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -8270,19 +8372,22 @@
         <v>549</v>
       </c>
       <c r="B77" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D77" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E77">
+        <v>229000</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -8290,19 +8395,22 @@
         <v>550</v>
       </c>
       <c r="B78" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D78" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E78">
+        <v>312000</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -8313,19 +8421,22 @@
         <v>411</v>
       </c>
       <c r="D79" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+      <c r="E79">
+        <v>1400000</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>183</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -8333,10 +8444,13 @@
         <v>560</v>
       </c>
       <c r="B80" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D80" t="s">
-        <v>453</v>
+        <v>659</v>
+      </c>
+      <c r="E80">
+        <v>2800000</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -8351,7 +8465,10 @@
         <v>452</v>
       </c>
       <c r="D81" t="s">
-        <v>662</v>
+        <v>659</v>
+      </c>
+      <c r="E81">
+        <v>3600000</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>107</v>
@@ -8370,9 +8487,6 @@
       <c r="B82" t="s">
         <v>451</v>
       </c>
-      <c r="D82" t="s">
-        <v>662</v>
-      </c>
       <c r="F82" s="4" t="s">
         <v>450</v>
       </c>
@@ -8388,10 +8502,7 @@
         <v>571</v>
       </c>
       <c r="B83" t="s">
-        <v>661</v>
-      </c>
-      <c r="D83" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>447</v>
@@ -8406,10 +8517,7 @@
         <v>940</v>
       </c>
       <c r="B84" t="s">
-        <v>660</v>
-      </c>
-      <c r="D84" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -8429,7 +8537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2 Q3:T78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Inventory Turns; TMA Harvest Report Changes
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="663">
   <si>
     <t>Abilene</t>
   </si>
@@ -2013,12 +2013,15 @@
   </si>
   <si>
     <t>CPC</t>
+  </si>
+  <si>
+    <t>CGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2837,7 +2840,7 @@
   </sheetPr>
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6534,7 +6537,7 @@
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -7782,7 +7785,7 @@
         <v>563</v>
       </c>
       <c r="D53" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E53">
         <v>1328500</v>
@@ -7814,7 +7817,7 @@
         <v>556</v>
       </c>
       <c r="D54" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E54">
         <v>400000</v>
@@ -7834,7 +7837,7 @@
         <v>555</v>
       </c>
       <c r="D55" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E55">
         <v>218560</v>
@@ -7860,7 +7863,7 @@
         <v>550</v>
       </c>
       <c r="D56" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E56">
         <v>993000</v>
@@ -7886,7 +7889,7 @@
         <v>367</v>
       </c>
       <c r="D57" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E57">
         <v>550800</v>
@@ -7912,7 +7915,7 @@
         <v>542</v>
       </c>
       <c r="D58" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E58">
         <v>345600</v>

</xml_diff>

<commit_message>
Updated the location capacities to include comma designation separator
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -16,7 +16,7 @@
     <sheet name="BranchData" sheetId="2" r:id="rId2"/>
     <sheet name="TMALocations" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="773">
   <si>
     <t>Abilene</t>
   </si>
@@ -2099,6 +2099,252 @@
   </si>
   <si>
     <t>185</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>716,000</t>
+  </si>
+  <si>
+    <t>813</t>
+  </si>
+  <si>
+    <t>30,000</t>
+  </si>
+  <si>
+    <t>1,216,000</t>
+  </si>
+  <si>
+    <t>577,000</t>
+  </si>
+  <si>
+    <t>1,740</t>
+  </si>
+  <si>
+    <t>551,000</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>1,581,000</t>
+  </si>
+  <si>
+    <t>288,000</t>
+  </si>
+  <si>
+    <t>764</t>
+  </si>
+  <si>
+    <t>32,000</t>
+  </si>
+  <si>
+    <t>790,000</t>
+  </si>
+  <si>
+    <t>250,700</t>
+  </si>
+  <si>
+    <t>699</t>
+  </si>
+  <si>
+    <t>64,000</t>
+  </si>
+  <si>
+    <t>1,689,669</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
+    <t>25,750</t>
+  </si>
+  <si>
+    <t>618,000</t>
+  </si>
+  <si>
+    <t>439,000</t>
+  </si>
+  <si>
+    <t>357,000</t>
+  </si>
+  <si>
+    <t>258,000</t>
+  </si>
+  <si>
+    <t>187,000</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>262,000</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>643,000</t>
+  </si>
+  <si>
+    <t>630</t>
+  </si>
+  <si>
+    <t>46,000</t>
+  </si>
+  <si>
+    <t>205,000</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>14,225</t>
+  </si>
+  <si>
+    <t>4,460,181</t>
+  </si>
+  <si>
+    <t>6,992</t>
+  </si>
+  <si>
+    <t>30,500</t>
+  </si>
+  <si>
+    <t>1,110,000</t>
+  </si>
+  <si>
+    <t>3,000</t>
+  </si>
+  <si>
+    <t>1,564</t>
+  </si>
+  <si>
+    <t>20,700</t>
+  </si>
+  <si>
+    <t>1,071</t>
+  </si>
+  <si>
+    <t>20,400</t>
+  </si>
+  <si>
+    <t>1,467,000</t>
+  </si>
+  <si>
+    <t>730</t>
+  </si>
+  <si>
+    <t>260,000</t>
+  </si>
+  <si>
+    <t>48,000</t>
+  </si>
+  <si>
+    <t>1,492</t>
+  </si>
+  <si>
+    <t>153,000</t>
+  </si>
+  <si>
+    <t>1,266,000</t>
+  </si>
+  <si>
+    <t>36,000</t>
+  </si>
+  <si>
+    <t>1,615,000</t>
+  </si>
+  <si>
+    <t>18,000</t>
+  </si>
+  <si>
+    <t>1,825,000</t>
+  </si>
+  <si>
+    <t>1,098</t>
+  </si>
+  <si>
+    <t>36,300</t>
+  </si>
+  <si>
+    <t>1,478,000</t>
+  </si>
+  <si>
+    <t>436,000</t>
+  </si>
+  <si>
+    <t>9,500</t>
+  </si>
+  <si>
+    <t>763</t>
+  </si>
+  <si>
+    <t>40,100</t>
+  </si>
+  <si>
+    <t>1,413,000</t>
+  </si>
+  <si>
+    <t>673</t>
+  </si>
+  <si>
+    <t>22,000</t>
+  </si>
+  <si>
+    <t>801,000</t>
+  </si>
+  <si>
+    <t>2,178,000</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>279,000</t>
+  </si>
+  <si>
+    <t>24,000</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>608,000</t>
+  </si>
+  <si>
+    <t>1,210</t>
+  </si>
+  <si>
+    <t>22,500</t>
+  </si>
+  <si>
+    <t>1,267,820</t>
+  </si>
+  <si>
+    <t>1,735</t>
+  </si>
+  <si>
+    <t>42,000</t>
+  </si>
+  <si>
+    <t>3,262,000</t>
+  </si>
+  <si>
+    <t>44,000</t>
+  </si>
+  <si>
+    <t>1,530</t>
+  </si>
+  <si>
+    <t>1,113,000</t>
+  </si>
+  <si>
+    <t>1,985,000</t>
+  </si>
+  <si>
+    <t>469,000</t>
   </si>
 </sst>
 </file>
@@ -2134,13 +2380,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2148,6 +2395,15 @@
   <dxfs count="14">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2168,16 +2424,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2228,16 +2475,16 @@
     <tableColumn id="9" name="Services"/>
     <tableColumn id="10" name="LocationCode"/>
     <tableColumn id="11" name="LocGLStr" dataDxfId="13"/>
-    <tableColumn id="20" name="TMA_BRANCH_NUMBER" dataDxfId="0"/>
-    <tableColumn id="15" name="LOCNCODE" dataDxfId="12"/>
-    <tableColumn id="19" name="AgLocationCode" dataDxfId="11"/>
-    <tableColumn id="12" name="Latitude" dataDxfId="10"/>
-    <tableColumn id="13" name="Longitude" dataDxfId="9"/>
-    <tableColumn id="14" name="Region" dataDxfId="8"/>
-    <tableColumn id="18" name="CapacityAppl" dataDxfId="7"/>
-    <tableColumn id="16" name="CapacityFert" dataDxfId="6"/>
-    <tableColumn id="17" name="CapacityFuel" dataDxfId="5"/>
-    <tableColumn id="22" name="CapacityGrain" dataDxfId="4"/>
+    <tableColumn id="20" name="TMA_BRANCH_NUMBER" dataDxfId="12"/>
+    <tableColumn id="15" name="LOCNCODE" dataDxfId="11"/>
+    <tableColumn id="19" name="AgLocationCode" dataDxfId="10"/>
+    <tableColumn id="12" name="Latitude" dataDxfId="9"/>
+    <tableColumn id="13" name="Longitude" dataDxfId="8"/>
+    <tableColumn id="14" name="Region" dataDxfId="7"/>
+    <tableColumn id="18" name="CapacityAppl" dataDxfId="3"/>
+    <tableColumn id="16" name="CapacityFert" dataDxfId="2"/>
+    <tableColumn id="17" name="CapacityFuel" dataDxfId="1"/>
+    <tableColumn id="22" name="CapacityGrain" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2252,9 +2499,9 @@
     <tableColumn id="3" name="TYPE"/>
     <tableColumn id="4" name="REGION"/>
     <tableColumn id="5" name="CAPACITY"/>
-    <tableColumn id="6" name="DisplayName" dataDxfId="3"/>
-    <tableColumn id="7" name="Address" dataDxfId="2"/>
-    <tableColumn id="8" name="Phone1" dataDxfId="1"/>
+    <tableColumn id="6" name="DisplayName" dataDxfId="6"/>
+    <tableColumn id="7" name="Address" dataDxfId="5"/>
+    <tableColumn id="8" name="Phone1" dataDxfId="4"/>
     <tableColumn id="9" name="Phone2"/>
     <tableColumn id="10" name="Phone3"/>
     <tableColumn id="11" name="Fax"/>
@@ -2341,6 +2588,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2376,6 +2640,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2909,9 +3190,7 @@
   </sheetPr>
   <dimension ref="A1:AG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3059,15 +3338,15 @@
         <v>-97.202228000000005</v>
       </c>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2">
-        <v>600</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>716000</v>
+      <c r="S2" s="4"/>
+      <c r="T2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>692</v>
       </c>
       <c r="AA2" t="s">
         <v>0</v>
@@ -3138,15 +3417,15 @@
         <v>-96.494437399999995</v>
       </c>
       <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2">
-        <v>813</v>
-      </c>
-      <c r="U3" s="2">
-        <v>30000</v>
-      </c>
-      <c r="V3" s="2">
-        <v>1216000</v>
+      <c r="S3" s="4"/>
+      <c r="T3" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -3191,15 +3470,15 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2">
-        <v>577000</v>
+      <c r="S4" s="4"/>
+      <c r="T4" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>696</v>
       </c>
       <c r="AA4" t="s">
         <v>2</v>
@@ -3270,15 +3549,15 @@
         <v>-97.592381799999998</v>
       </c>
       <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
-        <v>1740</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>551000</v>
+      <c r="S5" s="4"/>
+      <c r="T5" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>698</v>
       </c>
       <c r="AA5" t="s">
         <v>3</v>
@@ -3349,15 +3628,15 @@
         <v>-97.107370000000003</v>
       </c>
       <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2">
-        <v>304</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>1581000</v>
+      <c r="S6" s="4"/>
+      <c r="T6" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>700</v>
       </c>
       <c r="AA6" t="s">
         <v>4</v>
@@ -3399,15 +3678,15 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
-        <v>288000</v>
+      <c r="S7" s="4"/>
+      <c r="T7" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
@@ -3460,15 +3739,15 @@
         <v>-97.770600299999998</v>
       </c>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2">
-        <v>764</v>
-      </c>
-      <c r="U8" s="2">
-        <v>32000</v>
-      </c>
-      <c r="V8" s="2">
-        <v>790000</v>
+      <c r="S8" s="4"/>
+      <c r="T8" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>704</v>
       </c>
       <c r="AA8" t="s">
         <v>6</v>
@@ -3510,15 +3789,15 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2">
-        <v>250700</v>
-      </c>
-      <c r="V9" s="2">
-        <v>0</v>
+      <c r="S9" s="4"/>
+      <c r="T9" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
@@ -3571,15 +3850,15 @@
         <v>-96.886448299999998</v>
       </c>
       <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2">
-        <v>699</v>
-      </c>
-      <c r="U10" s="2">
-        <v>64000</v>
-      </c>
-      <c r="V10" s="2">
-        <v>1689669</v>
+      <c r="S10" s="4"/>
+      <c r="T10" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>708</v>
       </c>
       <c r="AA10" t="s">
         <v>7</v>
@@ -3642,10 +3921,10 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
       <c r="AA11" t="s">
         <v>107</v>
       </c>
@@ -3715,15 +3994,15 @@
         <v>-97.968699999999998</v>
       </c>
       <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2">
-        <v>677</v>
-      </c>
-      <c r="U12" s="2">
-        <v>25750</v>
-      </c>
-      <c r="V12" s="2">
-        <v>618000</v>
+      <c r="S12" s="4"/>
+      <c r="T12" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>711</v>
       </c>
       <c r="AA12" t="s">
         <v>8</v>
@@ -3769,10 +4048,10 @@
         <v>-97.666996100000006</v>
       </c>
       <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3803,15 +4082,15 @@
         <v>-97.664208700000003</v>
       </c>
       <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2">
-        <v>0</v>
-      </c>
-      <c r="U14" s="2">
-        <v>0</v>
-      </c>
-      <c r="V14" s="2">
-        <v>439000</v>
+      <c r="S14" s="4"/>
+      <c r="T14" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -3856,11 +4135,11 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2">
-        <v>357000</v>
+      <c r="S15" s="4"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1" t="s">
+        <v>713</v>
       </c>
       <c r="AA15" t="s">
         <v>114</v>
@@ -3929,15 +4208,15 @@
         <v>-97.618053500000002</v>
       </c>
       <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
-        <v>258000</v>
+      <c r="S16" s="4"/>
+      <c r="T16" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>714</v>
       </c>
       <c r="AA16" t="s">
         <v>10</v>
@@ -3981,10 +4260,10 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4028,15 +4307,15 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2">
-        <v>0</v>
-      </c>
-      <c r="U18" s="2">
-        <v>0</v>
-      </c>
-      <c r="V18" s="2">
-        <v>187000</v>
+      <c r="S18" s="4"/>
+      <c r="T18" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
@@ -4089,15 +4368,15 @@
         <v>-96.926252000000005</v>
       </c>
       <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2">
-        <v>250</v>
-      </c>
-      <c r="U19" s="2">
-        <v>0</v>
-      </c>
-      <c r="V19" s="2">
-        <v>262000</v>
+      <c r="S19" s="4"/>
+      <c r="T19" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>717</v>
       </c>
       <c r="AA19" t="s">
         <v>12</v>
@@ -4168,15 +4447,15 @@
         <v>-97.538265899999999</v>
       </c>
       <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2">
-        <v>299</v>
-      </c>
-      <c r="U20" s="2">
-        <v>30000</v>
-      </c>
-      <c r="V20" s="2">
-        <v>643000</v>
+      <c r="S20" s="4"/>
+      <c r="T20" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
@@ -4229,15 +4508,15 @@
         <v>-97.515514600000003</v>
       </c>
       <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2">
-        <v>630</v>
-      </c>
-      <c r="U21" s="2">
-        <v>46000</v>
-      </c>
-      <c r="V21" s="2">
-        <v>205000</v>
+      <c r="S21" s="4"/>
+      <c r="T21" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
@@ -4290,15 +4569,15 @@
         <v>-97.779943399999993</v>
       </c>
       <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2">
-        <v>92</v>
-      </c>
-      <c r="U22" s="2">
-        <v>14225</v>
-      </c>
-      <c r="V22" s="2">
-        <v>4460181</v>
+      <c r="S22" s="4"/>
+      <c r="T22" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>725</v>
       </c>
       <c r="AA22" t="s">
         <v>15</v>
@@ -4369,15 +4648,15 @@
         <v>-97.784899899999999</v>
       </c>
       <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2">
-        <v>6992</v>
-      </c>
-      <c r="U23" s="2">
-        <v>30500</v>
-      </c>
-      <c r="V23" s="2">
-        <v>1110000</v>
+      <c r="S23" s="4"/>
+      <c r="T23" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>728</v>
       </c>
       <c r="AA23" t="s">
         <v>16</v>
@@ -4421,10 +4700,10 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4472,15 +4751,15 @@
         <v>-96.948407000000003</v>
       </c>
       <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2">
-        <v>0</v>
-      </c>
-      <c r="U25" s="2">
-        <v>3000</v>
-      </c>
-      <c r="V25" s="2">
-        <v>0</v>
+      <c r="S25" s="4"/>
+      <c r="T25" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="AA25" t="s">
         <v>17</v>
@@ -4543,10 +4822,10 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -4571,10 +4850,10 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -4597,10 +4876,10 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -4648,15 +4927,15 @@
         <v>-97.774975999999995</v>
       </c>
       <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2">
-        <v>1564</v>
-      </c>
-      <c r="U29" s="2">
-        <v>20700</v>
-      </c>
-      <c r="V29" s="2">
-        <v>0</v>
+      <c r="S29" s="4"/>
+      <c r="T29" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="AA29" t="s">
         <v>19</v>
@@ -4727,15 +5006,15 @@
         <v>-97.671643000000003</v>
       </c>
       <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2">
-        <v>1071</v>
-      </c>
-      <c r="U30" s="2">
-        <v>20400</v>
-      </c>
-      <c r="V30" s="2">
-        <v>1467000</v>
+      <c r="S30" s="4"/>
+      <c r="T30" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>734</v>
       </c>
       <c r="AA30" t="s">
         <v>20</v>
@@ -4806,15 +5085,15 @@
         <v>-97.331413400000002</v>
       </c>
       <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2">
-        <v>730</v>
-      </c>
-      <c r="U31" s="2">
-        <v>0</v>
-      </c>
-      <c r="V31" s="2">
-        <v>260000</v>
+      <c r="S31" s="4"/>
+      <c r="T31" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
@@ -4842,10 +5121,10 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -4868,10 +5147,10 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -4919,15 +5198,15 @@
         <v>-96.557330500000006</v>
       </c>
       <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2">
-        <v>0</v>
-      </c>
-      <c r="U34" s="2">
-        <v>48000</v>
-      </c>
-      <c r="V34" s="2">
-        <v>0</v>
+      <c r="S34" s="4"/>
+      <c r="T34" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="AA34" t="s">
         <v>22</v>
@@ -4998,15 +5277,15 @@
         <v>-96.505954700000004</v>
       </c>
       <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2">
-        <v>1492</v>
-      </c>
-      <c r="U35" s="2">
-        <v>153000</v>
-      </c>
-      <c r="V35" s="2">
-        <v>1266000</v>
+      <c r="S35" s="4"/>
+      <c r="T35" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>740</v>
       </c>
       <c r="AA35" t="s">
         <v>152</v>
@@ -5077,15 +5356,15 @@
         <v>-97.834316099999995</v>
       </c>
       <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2">
-        <v>575</v>
-      </c>
-      <c r="U36" s="2">
-        <v>36000</v>
-      </c>
-      <c r="V36" s="2">
-        <v>1615000</v>
+      <c r="S36" s="4"/>
+      <c r="T36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>742</v>
       </c>
       <c r="AA36" t="s">
         <v>24</v>
@@ -5135,10 +5414,10 @@
         <v>-97.263819699999999</v>
       </c>
       <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -5186,10 +5465,10 @@
         <v>-97.666996100000006</v>
       </c>
       <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -5228,10 +5507,10 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
       <c r="AA39" t="s">
         <v>157</v>
       </c>
@@ -5288,10 +5567,10 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
       <c r="AA40" t="s">
         <v>160</v>
       </c>
@@ -5332,10 +5611,10 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -5385,15 +5664,15 @@
         <v>-97.668978899999999</v>
       </c>
       <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2">
-        <v>0</v>
-      </c>
-      <c r="U42" s="2">
-        <v>18000</v>
-      </c>
-      <c r="V42" s="2">
-        <v>1825000</v>
+      <c r="S42" s="4"/>
+      <c r="T42" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>744</v>
       </c>
       <c r="AA42" t="s">
         <v>166</v>
@@ -5457,10 +5736,10 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
       <c r="AA43" t="s">
         <v>79</v>
       </c>
@@ -5533,15 +5812,15 @@
         <v>-97.522767200000004</v>
       </c>
       <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2">
-        <v>1098</v>
-      </c>
-      <c r="U44" s="2">
-        <v>36300</v>
-      </c>
-      <c r="V44" s="2">
-        <v>1478000</v>
+      <c r="S44" s="4"/>
+      <c r="T44" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>747</v>
       </c>
       <c r="AA44" t="s">
         <v>174</v>
@@ -5597,10 +5876,10 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
       <c r="AA45" t="s">
         <v>169</v>
       </c>
@@ -5641,10 +5920,10 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -5686,15 +5965,15 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2">
-        <v>0</v>
-      </c>
-      <c r="U47" s="2">
-        <v>0</v>
-      </c>
-      <c r="V47" s="2">
-        <v>436000</v>
+      <c r="S47" s="4"/>
+      <c r="T47" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>748</v>
       </c>
       <c r="AA47" t="s">
         <v>27</v>
@@ -5736,15 +6015,15 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2">
-        <v>0</v>
-      </c>
-      <c r="U48" s="2">
-        <v>9500</v>
-      </c>
-      <c r="V48" s="2">
-        <v>0</v>
+      <c r="S48" s="4"/>
+      <c r="T48" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
@@ -5797,15 +6076,15 @@
         <v>-96.177394699999994</v>
       </c>
       <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2">
-        <v>763</v>
-      </c>
-      <c r="U49" s="2">
-        <v>40100</v>
-      </c>
-      <c r="V49" s="2">
-        <v>1413000</v>
+      <c r="S49" s="4"/>
+      <c r="T49" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>752</v>
       </c>
       <c r="AA49" t="s">
         <v>28</v>
@@ -5876,15 +6155,15 @@
         <v>-97.103965099999996</v>
       </c>
       <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2">
-        <v>673</v>
-      </c>
-      <c r="U50" s="2">
-        <v>22000</v>
-      </c>
-      <c r="V50" s="2">
-        <v>801000</v>
+      <c r="S50" s="4"/>
+      <c r="T50" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>755</v>
       </c>
       <c r="AA50" t="s">
         <v>29</v>
@@ -5930,10 +6209,10 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -5958,10 +6237,10 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -5982,10 +6261,10 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -6031,15 +6310,15 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-      <c r="S54" s="2"/>
-      <c r="T54" s="2">
-        <v>0</v>
-      </c>
-      <c r="U54" s="2">
-        <v>0</v>
-      </c>
-      <c r="V54" s="2">
-        <v>2178000</v>
+      <c r="S54" s="4"/>
+      <c r="T54" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>756</v>
       </c>
       <c r="AA54" t="s">
         <v>181</v>
@@ -6102,15 +6381,15 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2">
-        <v>52</v>
-      </c>
-      <c r="U55" s="2">
-        <v>0</v>
-      </c>
-      <c r="V55" s="2">
-        <v>279000</v>
+      <c r="S55" s="4"/>
+      <c r="T55" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.25">
@@ -6156,15 +6435,15 @@
         <v>-97.614002999999997</v>
       </c>
       <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2">
-        <v>0</v>
-      </c>
-      <c r="U56" s="2">
-        <v>24000</v>
-      </c>
-      <c r="V56" s="2">
-        <v>0</v>
+      <c r="S56" s="4"/>
+      <c r="T56" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="AA56" t="s">
         <v>189</v>
@@ -6235,15 +6514,15 @@
         <v>-97.374758999999997</v>
       </c>
       <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2">
-        <v>950</v>
-      </c>
-      <c r="U57" s="2">
-        <v>0</v>
-      </c>
-      <c r="V57" s="2">
-        <v>608000</v>
+      <c r="S57" s="4"/>
+      <c r="T57" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="U57" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>761</v>
       </c>
       <c r="AA57" t="s">
         <v>30</v>
@@ -6314,15 +6593,15 @@
         <v>-97.259965699999995</v>
       </c>
       <c r="R58" s="2"/>
-      <c r="S58" s="2"/>
-      <c r="T58" s="2">
-        <v>1210</v>
-      </c>
-      <c r="U58" s="2">
-        <v>22500</v>
-      </c>
-      <c r="V58" s="2">
-        <v>1267820</v>
+      <c r="S58" s="4"/>
+      <c r="T58" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>764</v>
       </c>
       <c r="AA58" t="s">
         <v>31</v>
@@ -6362,10 +6641,10 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -6417,15 +6696,15 @@
         <v>-97.229442399999996</v>
       </c>
       <c r="R60" s="2"/>
-      <c r="S60" s="2"/>
-      <c r="T60" s="2">
-        <v>1735</v>
-      </c>
-      <c r="U60" s="2">
-        <v>42000</v>
-      </c>
-      <c r="V60" s="2">
-        <v>3262000</v>
+      <c r="S60" s="4"/>
+      <c r="T60" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>767</v>
       </c>
       <c r="AA60" t="s">
         <v>32</v>
@@ -6492,15 +6771,15 @@
         <v>-96.410154700000007</v>
       </c>
       <c r="R61" s="2"/>
-      <c r="S61" s="2"/>
-      <c r="T61" s="2">
-        <v>21</v>
-      </c>
-      <c r="U61" s="2">
-        <v>44000</v>
-      </c>
-      <c r="V61" s="2">
-        <v>0</v>
+      <c r="S61" s="4"/>
+      <c r="T61" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="U61" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="AA61" t="s">
         <v>33</v>
@@ -6571,15 +6850,15 @@
         <v>-97.150157199999995</v>
       </c>
       <c r="R62" s="2"/>
-      <c r="S62" s="2"/>
-      <c r="T62" s="2">
-        <v>1530</v>
-      </c>
-      <c r="U62" s="2">
-        <v>0</v>
-      </c>
-      <c r="V62" s="2">
-        <v>1113000</v>
+      <c r="S62" s="4"/>
+      <c r="T62" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>770</v>
       </c>
       <c r="AA62" t="s">
         <v>34</v>
@@ -6640,15 +6919,15 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-      <c r="S63" s="2"/>
-      <c r="T63" s="2">
-        <v>0</v>
-      </c>
-      <c r="U63" s="2">
-        <v>0</v>
-      </c>
-      <c r="V63" s="2">
-        <v>1985000</v>
+      <c r="S63" s="4"/>
+      <c r="T63" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U63" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>771</v>
       </c>
       <c r="AA63" t="s">
         <v>203</v>
@@ -6711,15 +6990,15 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
-      <c r="S64" s="2"/>
-      <c r="T64" s="2">
-        <v>0</v>
-      </c>
-      <c r="U64" s="2">
-        <v>0</v>
-      </c>
-      <c r="V64" s="2">
-        <v>469000</v>
+      <c r="S64" s="4"/>
+      <c r="T64" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U64" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="V64" s="1" t="s">
+        <v>772</v>
       </c>
       <c r="AA64" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Updated locations with missing lat/long values to show up on the MKC Location map; inactivated Conway
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="774">
   <si>
     <t>Abilene</t>
   </si>
@@ -2345,6 +2345,9 @@
   </si>
   <si>
     <t>469,000</t>
+  </si>
+  <si>
+    <t>38-798699</t>
   </si>
 </sst>
 </file>
@@ -2394,6 +2397,15 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -2404,15 +2416,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2481,10 +2484,10 @@
     <tableColumn id="12" name="Latitude" dataDxfId="9"/>
     <tableColumn id="13" name="Longitude" dataDxfId="8"/>
     <tableColumn id="14" name="Region" dataDxfId="7"/>
-    <tableColumn id="18" name="CapacityAppl" dataDxfId="3"/>
-    <tableColumn id="16" name="CapacityFert" dataDxfId="2"/>
-    <tableColumn id="17" name="CapacityFuel" dataDxfId="1"/>
-    <tableColumn id="22" name="CapacityGrain" dataDxfId="0"/>
+    <tableColumn id="18" name="CapacityAppl" dataDxfId="6"/>
+    <tableColumn id="16" name="CapacityFert" dataDxfId="5"/>
+    <tableColumn id="17" name="CapacityFuel" dataDxfId="4"/>
+    <tableColumn id="22" name="CapacityGrain" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2499,9 +2502,9 @@
     <tableColumn id="3" name="TYPE"/>
     <tableColumn id="4" name="REGION"/>
     <tableColumn id="5" name="CAPACITY"/>
-    <tableColumn id="6" name="DisplayName" dataDxfId="6"/>
-    <tableColumn id="7" name="Address" dataDxfId="5"/>
-    <tableColumn id="8" name="Phone1" dataDxfId="4"/>
+    <tableColumn id="6" name="DisplayName" dataDxfId="2"/>
+    <tableColumn id="7" name="Address" dataDxfId="1"/>
+    <tableColumn id="8" name="Phone1" dataDxfId="0"/>
     <tableColumn id="9" name="Phone2"/>
     <tableColumn id="10" name="Phone3"/>
     <tableColumn id="11" name="Fax"/>
@@ -3467,8 +3470,12 @@
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>-97.755188000000004</v>
+      </c>
       <c r="R4" s="2"/>
       <c r="S4" s="4"/>
       <c r="T4" s="1" t="s">
@@ -3675,8 +3682,12 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="P7" s="2">
+        <v>38.629404000000001</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>-97.615026999999998</v>
+      </c>
       <c r="R7" s="2"/>
       <c r="S7" s="4"/>
       <c r="T7" s="1" t="s">
@@ -3918,8 +3929,12 @@
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="P11" s="2">
+        <v>38.378869999999999</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>-97.470513999999994</v>
+      </c>
       <c r="R11" s="2"/>
       <c r="S11" s="4"/>
       <c r="T11" s="1"/>
@@ -4058,7 +4073,7 @@
         <v>284</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>260</v>
@@ -4132,8 +4147,12 @@
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="P15" s="2">
+        <v>38.9670597</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>-97.762475199999997</v>
+      </c>
       <c r="R15" s="2"/>
       <c r="S15" s="4"/>
       <c r="T15" s="1"/>
@@ -4202,10 +4221,10 @@
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="2">
-        <v>38.289623200000001</v>
+        <v>38.290137999999999</v>
       </c>
       <c r="Q16" s="2">
-        <v>-97.618053500000002</v>
+        <v>-97.625752000000006</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="4"/>
@@ -4304,8 +4323,12 @@
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="P18" s="2">
+        <v>38.672823000000001</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>-97.760738200000006</v>
+      </c>
       <c r="R18" s="2"/>
       <c r="S18" s="4"/>
       <c r="T18" s="1" t="s">
@@ -4502,10 +4525,10 @@
         <v>257</v>
       </c>
       <c r="P21" s="2">
-        <v>38.205322600000002</v>
+        <v>38.249427099999998</v>
       </c>
       <c r="Q21" s="2">
-        <v>-97.515514600000003</v>
+        <v>-97.337304200000005</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="4"/>
@@ -4819,8 +4842,12 @@
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
+      <c r="P26" s="2">
+        <v>38.441087199999998</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>-97.677783700000006</v>
+      </c>
       <c r="R26" s="2"/>
       <c r="S26" s="4"/>
       <c r="T26" s="1"/>
@@ -5962,8 +5989,12 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
+      <c r="P47" s="2">
+        <v>38.065479000000003</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>-97.345708000000002</v>
+      </c>
       <c r="R47" s="2"/>
       <c r="S47" s="4"/>
       <c r="T47" s="1" t="s">
@@ -6307,8 +6338,12 @@
         <v>332</v>
       </c>
       <c r="O54" s="1"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
+      <c r="P54" s="2">
+        <v>38.266167000000003</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>-98.200824999999995</v>
+      </c>
       <c r="R54" s="2"/>
       <c r="S54" s="4"/>
       <c r="T54" s="1" t="s">
@@ -6378,8 +6413,12 @@
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
+      <c r="P55" s="2">
+        <v>38.551245999999999</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>-97.429237000000001</v>
+      </c>
       <c r="R55" s="2"/>
       <c r="S55" s="4"/>
       <c r="T55" s="1" t="s">
@@ -6916,8 +6955,12 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
+      <c r="P63" s="2">
+        <v>37.739190899999997</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>-97.329066100000006</v>
+      </c>
       <c r="R63" s="2"/>
       <c r="S63" s="4"/>
       <c r="T63" s="1" t="s">
@@ -6987,8 +7030,12 @@
       </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
+      <c r="P64" s="2">
+        <v>38.385244999999998</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>-97.909503999999998</v>
+      </c>
       <c r="R64" s="2"/>
       <c r="S64" s="4"/>
       <c r="T64" s="1" t="s">

</xml_diff>

<commit_message>
Updated Seasonal Flags and geolocation for McPherson Energy
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="773">
   <si>
     <t>Abilene</t>
   </si>
@@ -3808,6 +3808,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
       <c r="K9">
         <v>34</v>
       </c>
@@ -4067,6 +4070,9 @@
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
       <c r="K13">
         <v>36</v>
       </c>
@@ -4096,6 +4102,9 @@
       </c>
       <c r="B14">
         <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
       </c>
       <c r="K14">
         <v>260</v>
@@ -4284,6 +4293,9 @@
       </c>
       <c r="B17">
         <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
       </c>
       <c r="K17">
         <v>305</v>
@@ -4729,6 +4741,9 @@
       <c r="B24">
         <v>1</v>
       </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
       <c r="K24">
         <v>430</v>
       </c>
@@ -4883,6 +4898,9 @@
       <c r="B27">
         <v>1</v>
       </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
       <c r="K27">
         <v>480</v>
       </c>
@@ -4911,6 +4929,9 @@
       <c r="B28">
         <v>0</v>
       </c>
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
       <c r="K28">
         <v>500</v>
       </c>
@@ -5152,6 +5173,9 @@
       <c r="B32">
         <v>1</v>
       </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
       <c r="K32">
         <v>570</v>
       </c>
@@ -5181,6 +5205,9 @@
       </c>
       <c r="B33">
         <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>115</v>
       </c>
       <c r="K33">
         <v>40</v>
@@ -5441,6 +5468,9 @@
       <c r="B37">
         <v>1</v>
       </c>
+      <c r="C37" t="s">
+        <v>115</v>
+      </c>
       <c r="K37">
         <v>600</v>
       </c>
@@ -5508,10 +5538,10 @@
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="2">
-        <v>38.4475148</v>
+        <v>38.3728713</v>
       </c>
       <c r="Q38" s="2">
-        <v>-97.666996100000006</v>
+        <v>-97.688086499999997</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="4"/>
@@ -5645,6 +5675,9 @@
       </c>
       <c r="B41">
         <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>115</v>
       </c>
       <c r="K41">
         <v>32</v>
@@ -5955,6 +5988,9 @@
       <c r="B46">
         <v>1</v>
       </c>
+      <c r="C46" t="s">
+        <v>115</v>
+      </c>
       <c r="K46">
         <v>680</v>
       </c>
@@ -6054,6 +6090,9 @@
       <c r="B48">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>115</v>
+      </c>
       <c r="K48">
         <v>682</v>
       </c>
@@ -6244,6 +6283,9 @@
       <c r="B51">
         <v>0</v>
       </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
       <c r="K51">
         <v>720</v>
       </c>
@@ -6274,6 +6316,9 @@
       <c r="B52">
         <v>1</v>
       </c>
+      <c r="C52" t="s">
+        <v>115</v>
+      </c>
       <c r="K52">
         <v>50</v>
       </c>
@@ -6301,6 +6346,9 @@
       </c>
       <c r="B53">
         <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>115</v>
       </c>
       <c r="K53">
         <v>740</v>
@@ -6689,6 +6737,9 @@
       </c>
       <c r="B59">
         <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
       </c>
       <c r="K59">
         <v>18</v>

</xml_diff>

<commit_message>
Updated sort for Midwest Feeders locations
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -2628,6 +2628,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M92" totalsRowShown="0">
   <autoFilter ref="A1:M92"/>
+  <sortState ref="A2:M92">
+    <sortCondition ref="A2:A92"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="BRANCH_NUMBER"/>
     <tableColumn id="2" name="BRANCH_NAME"/>
@@ -9279,195 +9282,195 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>940</v>
+        <v>630</v>
       </c>
       <c r="B84" t="s">
-        <v>642</v>
-      </c>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
+        <v>778</v>
+      </c>
+      <c r="D84" t="s">
+        <v>786</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="H84" t="s">
+        <v>796</v>
+      </c>
+      <c r="K84" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B85" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D85" t="s">
         <v>786</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>795</v>
-      </c>
-      <c r="H85" t="s">
-        <v>796</v>
+        <v>800</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>798</v>
       </c>
       <c r="K85" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B86" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D86" t="s">
         <v>786</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>798</v>
-      </c>
-      <c r="K86" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B87" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D87" t="s">
         <v>786</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>802</v>
+        <v>804</v>
+      </c>
+      <c r="K87" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="B88" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D88" t="s">
         <v>786</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="K88" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B89" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D89" t="s">
         <v>786</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="K89" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B90" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="D90" t="s">
         <v>786</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="K90" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B91" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D91" t="s">
         <v>786</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="K91" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>650</v>
+        <v>940</v>
       </c>
       <c r="B92" t="s">
-        <v>785</v>
-      </c>
-      <c r="D92" t="s">
-        <v>786</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>794</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>815</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>816</v>
-      </c>
-      <c r="K92" t="s">
-        <v>817</v>
-      </c>
+        <v>642</v>
+      </c>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
add p ag to financials
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -2954,14 +2954,14 @@
       <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3185,17 +3185,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>167</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>179</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>200</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -3346,36 +3346,36 @@
   </sheetPr>
   <dimension ref="A1:AG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="40.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="15" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="40.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="15" width="14.5546875" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>67017</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>67522</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>288</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>67428</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>281</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -4468,7 +4468,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -4915,7 +4915,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>67443</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -5041,7 +5041,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>316</v>
       </c>
@@ -5072,7 +5072,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -5101,7 +5101,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>67456</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>284</v>
       </c>
@@ -5349,7 +5349,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -5378,7 +5378,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>150</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>67464</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>336</v>
       </c>
@@ -5644,7 +5644,7 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -5695,7 +5695,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>155</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>287</v>
       </c>
@@ -5844,7 +5844,7 @@
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>164</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>167</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>285</v>
       </c>
@@ -6156,7 +6156,7 @@
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>286</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>319</v>
       </c>
@@ -6455,7 +6455,7 @@
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>314</v>
       </c>
@@ -6478,15 +6478,19 @@
       <c r="O52" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
+      <c r="P52" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>0</v>
+      </c>
       <c r="R52" s="2"/>
       <c r="S52" s="4"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>321</v>
       </c>
@@ -6513,7 +6517,7 @@
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -6590,7 +6594,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>184</v>
       </c>
@@ -6647,7 +6651,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>187</v>
       </c>
@@ -6719,7 +6723,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -6798,7 +6802,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -6877,7 +6881,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>309</v>
       </c>
@@ -6904,7 +6908,7 @@
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -6983,7 +6987,7 @@
         <v>67151</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -7058,7 +7062,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -7137,7 +7141,7 @@
         <v>67154</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>200</v>
       </c>
@@ -7210,7 +7214,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>35</v>
       </c>
@@ -7307,21 +7311,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>640</v>
       </c>
@@ -7362,7 +7366,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11</v>
       </c>
@@ -7391,7 +7395,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>13</v>
       </c>
@@ -7404,7 +7408,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>21</v>
       </c>
@@ -7430,7 +7434,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>31</v>
       </c>
@@ -7459,7 +7463,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>32</v>
       </c>
@@ -7478,7 +7482,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>41</v>
       </c>
@@ -7495,7 +7499,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>61</v>
       </c>
@@ -7524,7 +7528,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>71</v>
       </c>
@@ -7556,7 +7560,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>81</v>
       </c>
@@ -7579,7 +7583,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>91</v>
       </c>
@@ -7605,7 +7609,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>101</v>
       </c>
@@ -7628,7 +7632,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>111</v>
       </c>
@@ -7654,7 +7658,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>121</v>
       </c>
@@ -7680,7 +7684,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>131</v>
       </c>
@@ -7709,7 +7713,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>141</v>
       </c>
@@ -7732,7 +7736,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>151</v>
       </c>
@@ -7758,7 +7762,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>161</v>
       </c>
@@ -7781,7 +7785,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>171</v>
       </c>
@@ -7807,7 +7811,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>181</v>
       </c>
@@ -7827,7 +7831,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>182</v>
       </c>
@@ -7845,7 +7849,7 @@
       <c r="H21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>183</v>
       </c>
@@ -7871,7 +7875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>185</v>
       </c>
@@ -7888,7 +7892,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>187</v>
       </c>
@@ -7911,7 +7915,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>188</v>
       </c>
@@ -7928,7 +7932,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>190</v>
       </c>
@@ -7946,7 +7950,7 @@
       <c r="H26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>191</v>
       </c>
@@ -7972,7 +7976,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>192</v>
       </c>
@@ -8001,7 +8005,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>193</v>
       </c>
@@ -8027,7 +8031,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>194</v>
       </c>
@@ -8053,7 +8057,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>195</v>
       </c>
@@ -8079,7 +8083,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>196</v>
       </c>
@@ -8105,7 +8109,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>197</v>
       </c>
@@ -8123,7 +8127,7 @@
       <c r="H33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>198</v>
       </c>
@@ -8146,7 +8150,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>199</v>
       </c>
@@ -8164,7 +8168,7 @@
       <c r="H35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>201</v>
       </c>
@@ -8175,7 +8179,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>205</v>
       </c>
@@ -8198,7 +8202,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>212</v>
       </c>
@@ -8227,7 +8231,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>215</v>
       </c>
@@ -8246,7 +8250,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>222</v>
       </c>
@@ -8272,7 +8276,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>242</v>
       </c>
@@ -8298,7 +8302,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>245</v>
       </c>
@@ -8316,7 +8320,7 @@
       <c r="H42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>252</v>
       </c>
@@ -8342,7 +8346,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>262</v>
       </c>
@@ -8368,7 +8372,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>272</v>
       </c>
@@ -8394,7 +8398,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>282</v>
       </c>
@@ -8412,7 +8416,7 @@
       <c r="H46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>291</v>
       </c>
@@ -8430,7 +8434,7 @@
       <c r="H47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>292</v>
       </c>
@@ -8456,7 +8460,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>293</v>
       </c>
@@ -8479,7 +8483,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>294</v>
       </c>
@@ -8502,7 +8506,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>295</v>
       </c>
@@ -8525,7 +8529,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>296</v>
       </c>
@@ -8542,7 +8546,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>311</v>
       </c>
@@ -8574,7 +8578,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>315</v>
       </c>
@@ -8594,7 +8598,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>331</v>
       </c>
@@ -8620,7 +8624,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>341</v>
       </c>
@@ -8646,7 +8650,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>351</v>
       </c>
@@ -8672,7 +8676,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>361</v>
       </c>
@@ -8693,7 +8697,7 @@
       </c>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>432</v>
       </c>
@@ -8710,7 +8714,7 @@
       <c r="G59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>433</v>
       </c>
@@ -8736,7 +8740,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>442</v>
       </c>
@@ -8762,7 +8766,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>443</v>
       </c>
@@ -8788,7 +8792,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>445</v>
       </c>
@@ -8806,7 +8810,7 @@
       <c r="H63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>447</v>
       </c>
@@ -8829,7 +8833,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>510</v>
       </c>
@@ -8855,7 +8859,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>520</v>
       </c>
@@ -8881,7 +8885,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>530</v>
       </c>
@@ -8907,7 +8911,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>540</v>
       </c>
@@ -8933,7 +8937,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>541</v>
       </c>
@@ -8956,7 +8960,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>542</v>
       </c>
@@ -8982,7 +8986,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>543</v>
       </c>
@@ -9008,7 +9012,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>544</v>
       </c>
@@ -9034,7 +9038,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>545</v>
       </c>
@@ -9057,7 +9061,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>546</v>
       </c>
@@ -9083,7 +9087,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>547</v>
       </c>
@@ -9109,7 +9113,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>548</v>
       </c>
@@ -9135,7 +9139,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>549</v>
       </c>
@@ -9158,7 +9162,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>550</v>
       </c>
@@ -9181,7 +9185,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>551</v>
       </c>
@@ -9207,7 +9211,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>560</v>
       </c>
@@ -9225,7 +9229,7 @@
       <c r="H80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>561</v>
       </c>
@@ -9248,7 +9252,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>570</v>
       </c>
@@ -9265,7 +9269,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>571</v>
       </c>
@@ -9280,7 +9284,7 @@
       </c>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>630</v>
       </c>
@@ -9303,7 +9307,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>632</v>
       </c>
@@ -9326,7 +9330,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>634</v>
       </c>
@@ -9346,7 +9350,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>636</v>
       </c>
@@ -9369,7 +9373,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>642</v>
       </c>
@@ -9392,7 +9396,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>644</v>
       </c>
@@ -9415,7 +9419,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>646</v>
       </c>
@@ -9438,7 +9442,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>650</v>
       </c>
@@ -9461,7 +9465,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>940</v>
       </c>

</xml_diff>

<commit_message>
changes to location file
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dashboardProd1\c$\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="818">
   <si>
     <t>Abilene</t>
   </si>
@@ -2584,8 +2584,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblLocationImages" displayName="tblLocationImages" ref="A1:B47" totalsRowShown="0">
-  <autoFilter ref="A1:B47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblLocationImages" displayName="tblLocationImages" ref="A1:B48" totalsRowShown="0">
+  <autoFilter ref="A1:B48"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Location"/>
     <tableColumn id="2" name="Image"/>
@@ -2947,11 +2947,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3253,81 +3253,89 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s">
-        <v>775</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B39" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>777</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>35</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3347,7 +3355,7 @@
   <dimension ref="A1:AG64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6465,6 +6473,24 @@
       <c r="C52" t="s">
         <v>114</v>
       </c>
+      <c r="D52" t="s">
+        <v>131</v>
+      </c>
+      <c r="F52" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52">
+        <v>67546</v>
+      </c>
+      <c r="I52" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52" t="s">
+        <v>314</v>
+      </c>
       <c r="K52">
         <v>50</v>
       </c>
@@ -6479,16 +6505,22 @@
         <v>428</v>
       </c>
       <c r="P52" s="2">
-        <v>0</v>
+        <v>38.289691599999998</v>
       </c>
       <c r="Q52" s="2">
-        <v>0</v>
+        <v>-97.779943399999993</v>
       </c>
       <c r="R52" s="2"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
+      <c r="T52" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" t="s">

</xml_diff>

<commit_message>
Updated MKC location spreadsheet with 035 Manhattan Bulk Fuel
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dashboardProd1\c$\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="823">
   <si>
     <t>Abilene</t>
   </si>
@@ -2480,6 +2480,21 @@
   </si>
   <si>
     <t>(417) 448-5987</t>
+  </si>
+  <si>
+    <t>Manhattan Bulk Fuel</t>
+  </si>
+  <si>
+    <t>3384 Excel Rd</t>
+  </si>
+  <si>
+    <t>Bulk fuel and oil</t>
+  </si>
+  <si>
+    <t>MHBULK</t>
+  </si>
+  <si>
+    <t>Manhattan Builk Fuel</t>
   </si>
 </sst>
 </file>
@@ -2584,8 +2599,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblLocationImages" displayName="tblLocationImages" ref="A1:B48" totalsRowShown="0">
-  <autoFilter ref="A1:B48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblLocationImages" displayName="tblLocationImages" ref="A1:B49" totalsRowShown="0">
+  <autoFilter ref="A1:B49"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Location"/>
     <tableColumn id="2" name="Image"/>
@@ -2595,8 +2610,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblLocation" displayName="tblLocation" ref="A1:V64" totalsRowShown="0">
-  <autoFilter ref="A1:V64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblLocation" displayName="tblLocation" ref="A1:V65" totalsRowShown="0">
+  <autoFilter ref="A1:V65"/>
   <tableColumns count="22">
     <tableColumn id="1" name="Location"/>
     <tableColumn id="23" name="Active"/>
@@ -2947,21 +2962,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2969,7 +2984,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2977,7 +2992,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2985,7 +3000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2993,7 +3008,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3001,7 +3016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +3024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3017,7 +3032,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3025,7 +3040,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3033,7 +3048,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3041,7 +3056,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3049,7 +3064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -3057,7 +3072,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3065,7 +3080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3073,7 +3088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3081,7 +3096,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3104,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3097,7 +3112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3105,7 +3120,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3113,7 +3128,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3121,7 +3136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3129,7 +3144,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3137,7 +3152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3145,7 +3160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3153,7 +3168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3161,181 +3176,189 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>822</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>164</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>167</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>314</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>179</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>184</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>187</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>32</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>34</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>200</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>35</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3352,38 +3375,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG64"/>
+  <dimension ref="A1:AG65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
-    <col min="14" max="15" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3454,7 +3477,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3533,7 +3556,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3594,7 +3617,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3669,7 +3692,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3748,7 +3771,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3827,7 +3850,7 @@
         <v>67017</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3884,7 +3907,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3963,7 +3986,7 @@
         <v>67522</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>288</v>
       </c>
@@ -3998,7 +4021,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4077,7 +4100,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -4146,7 +4169,7 @@
         <v>67428</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4225,7 +4248,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -4254,7 +4277,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>281</v>
       </c>
@@ -4297,7 +4320,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4368,7 +4391,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4445,7 +4468,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -4476,7 +4499,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4533,7 +4556,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4612,7 +4635,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4673,7 +4696,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4734,7 +4757,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -4813,7 +4836,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -4892,7 +4915,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -4923,7 +4946,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -4998,7 +5021,7 @@
         <v>67443</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -5049,7 +5072,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>316</v>
       </c>
@@ -5080,7 +5103,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -5109,7 +5132,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5184,7 +5207,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -5263,7 +5286,7 @@
         <v>67456</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -5324,7 +5347,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>284</v>
       </c>
@@ -5357,7 +5380,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -5386,7 +5409,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -5461,9 +5484,9 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>818</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5472,7 +5495,7 @@
         <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>819</v>
       </c>
       <c r="F35" t="s">
         <v>23</v>
@@ -5483,66 +5506,31 @@
       <c r="H35">
         <v>66502</v>
       </c>
-      <c r="I35" t="s">
-        <v>149</v>
-      </c>
       <c r="J35" t="s">
-        <v>100</v>
+        <v>820</v>
       </c>
       <c r="K35">
-        <v>575</v>
+        <v>34</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>680</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="P35" s="2">
-        <v>39.192815099999997</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>-96.505954700000004</v>
-      </c>
+        <v>821</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="4"/>
-      <c r="T35" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="AA35" t="s">
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>150</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>375</v>
-      </c>
-      <c r="AE35" t="s">
-        <v>269</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG35" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>24</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -5551,77 +5539,77 @@
         <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" t="s">
         <v>82</v>
       </c>
       <c r="H36">
-        <v>67464</v>
+        <v>66502</v>
       </c>
       <c r="I36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J36" t="s">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>657</v>
+        <v>680</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P36" s="2">
-        <v>38.557795300000002</v>
+        <v>39.192815099999997</v>
       </c>
       <c r="Q36" s="2">
-        <v>-97.834316099999995</v>
+        <v>-96.505954700000004</v>
       </c>
       <c r="R36" s="2"/>
       <c r="S36" s="4"/>
       <c r="T36" s="1" t="s">
-        <v>226</v>
+        <v>735</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="AA36" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="AB36" t="s">
         <v>339</v>
       </c>
       <c r="AC36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AE36" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="AF36" t="s">
         <v>82</v>
       </c>
-      <c r="AG36">
-        <v>67464</v>
-      </c>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>336</v>
+        <v>24</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -5629,32 +5617,78 @@
       <c r="C37" t="s">
         <v>114</v>
       </c>
+      <c r="D37" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37">
+        <v>67464</v>
+      </c>
+      <c r="I37" t="s">
+        <v>154</v>
+      </c>
+      <c r="J37" t="s">
+        <v>100</v>
+      </c>
       <c r="K37">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>298</v>
+        <v>227</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>669</v>
+        <v>657</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>335</v>
+        <v>259</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
+        <v>424</v>
+      </c>
+      <c r="P37" s="2">
+        <v>38.557795300000002</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>-97.834316099999995</v>
+      </c>
       <c r="R37" s="2"/>
       <c r="S37" s="4"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T37" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>377</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG37">
+        <v>67464</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>336</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -5662,50 +5696,32 @@
       <c r="C38" t="s">
         <v>114</v>
       </c>
-      <c r="D38" t="s">
-        <v>161</v>
-      </c>
-      <c r="F38" t="s">
-        <v>119</v>
-      </c>
-      <c r="G38" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38">
-        <v>67460</v>
-      </c>
-      <c r="I38" t="s">
-        <v>162</v>
-      </c>
-      <c r="J38" t="s">
-        <v>163</v>
-      </c>
       <c r="K38">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="M38" s="1"/>
+        <v>298</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>669</v>
+      </c>
       <c r="N38" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="O38" s="1"/>
-      <c r="P38" s="2">
-        <v>38.372259999999997</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>-97.685670999999999</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="4"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -5714,7 +5730,7 @@
         <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F39" t="s">
         <v>119</v>
@@ -5726,46 +5742,37 @@
         <v>67460</v>
       </c>
       <c r="I39" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="J39" t="s">
-        <v>84</v>
-      </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="N39" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="K39">
+        <v>30</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="O39" s="1"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
+      <c r="P39" s="2">
+        <v>38.372259999999997</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>-97.685670999999999</v>
+      </c>
       <c r="R39" s="2"/>
       <c r="S39" s="4"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
-      <c r="AA39" t="s">
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>155</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>378</v>
-      </c>
-      <c r="AE39" t="s">
-        <v>270</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG39" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>158</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -5774,7 +5781,7 @@
         <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
         <v>119</v>
@@ -5786,14 +5793,14 @@
         <v>67460</v>
       </c>
       <c r="I40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J40" t="s">
         <v>84</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -5805,13 +5812,13 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="AA40" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AB40" t="s">
         <v>339</v>
       </c>
       <c r="AC40" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AE40" t="s">
         <v>270</v>
@@ -5820,12 +5827,12 @@
         <v>82</v>
       </c>
       <c r="AG40" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>287</v>
+        <v>158</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -5833,16 +5840,29 @@
       <c r="C41" t="s">
         <v>114</v>
       </c>
-      <c r="K41">
-        <v>32</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1" t="s">
-        <v>323</v>
-      </c>
+      <c r="D41" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" t="s">
+        <v>82</v>
+      </c>
+      <c r="H41">
+        <v>67460</v>
+      </c>
+      <c r="I41" t="s">
+        <v>160</v>
+      </c>
+      <c r="J41" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
@@ -5851,10 +5871,28 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA41" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>380</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>287</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -5862,76 +5900,28 @@
       <c r="C42" t="s">
         <v>114</v>
       </c>
-      <c r="D42" t="s">
-        <v>165</v>
-      </c>
-      <c r="F42" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42">
-        <v>67460</v>
-      </c>
-      <c r="I42" t="s">
-        <v>166</v>
-      </c>
-      <c r="J42" t="s">
-        <v>84</v>
-      </c>
       <c r="K42">
-        <v>620</v>
+        <v>32</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>687</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="M42" s="1"/>
       <c r="N42" s="1" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="O42" s="1"/>
-      <c r="P42" s="2">
-        <v>38.372224000000003</v>
-      </c>
-      <c r="Q42" s="2">
-        <v>-97.668978899999999</v>
-      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="4"/>
-      <c r="T42" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="U42" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="AA42" t="s">
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>164</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC42" t="s">
-        <v>382</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>270</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG42" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>78</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -5940,64 +5930,75 @@
         <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
-      </c>
-      <c r="E43" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="F43" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="G43" t="s">
         <v>82</v>
       </c>
       <c r="H43">
-        <v>67107</v>
+        <v>67460</v>
       </c>
       <c r="I43" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="J43" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="K43">
-        <v>10</v>
+        <v>620</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="O43" s="1"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
+      <c r="P43" s="2">
+        <v>38.372224000000003</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>-97.668978899999999</v>
+      </c>
       <c r="R43" s="2"/>
       <c r="S43" s="4"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
+      <c r="T43" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>741</v>
+      </c>
       <c r="AA43" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
       <c r="AB43" t="s">
         <v>339</v>
       </c>
       <c r="AC43" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AE43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AF43" t="s">
         <v>82</v>
       </c>
       <c r="AG43" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -6021,45 +6022,29 @@
         <v>67107</v>
       </c>
       <c r="I44" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="J44" t="s">
         <v>100</v>
       </c>
       <c r="K44">
-        <v>640</v>
+        <v>10</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="P44" s="2">
-        <v>38.202722299999998</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>-97.522767200000004</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="4"/>
-      <c r="T44" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>744</v>
-      </c>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
       <c r="AA44" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="AB44" t="s">
         <v>339</v>
@@ -6077,9 +6062,9 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -6088,7 +6073,10 @@
         <v>114</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
       </c>
       <c r="F45" t="s">
         <v>26</v>
@@ -6100,30 +6088,51 @@
         <v>67107</v>
       </c>
       <c r="I45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J45" t="s">
-        <v>171</v>
-      </c>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="K45">
+        <v>640</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="P45" s="2">
+        <v>38.202722299999998</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>-97.522767200000004</v>
+      </c>
       <c r="R45" s="2"/>
       <c r="S45" s="4"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
+      <c r="T45" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>744</v>
+      </c>
       <c r="AA45" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="AB45" t="s">
         <v>339</v>
       </c>
       <c r="AC45" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AE45" t="s">
         <v>271</v>
@@ -6132,12 +6141,12 @@
         <v>82</v>
       </c>
       <c r="AG45" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>285</v>
+        <v>167</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -6145,15 +6154,26 @@
       <c r="C46" t="s">
         <v>114</v>
       </c>
-      <c r="K46">
-        <v>680</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>681</v>
-      </c>
+      <c r="D46" t="s">
+        <v>168</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46">
+        <v>67107</v>
+      </c>
+      <c r="I46" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" t="s">
+        <v>171</v>
+      </c>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="2"/>
@@ -6163,118 +6183,130 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA46" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>271</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>285</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" t="s">
-        <v>173</v>
-      </c>
-      <c r="F47" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" t="s">
-        <v>82</v>
-      </c>
-      <c r="H47">
-        <v>67117</v>
-      </c>
-      <c r="I47" t="s">
-        <v>174</v>
-      </c>
-      <c r="J47" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="K47">
-        <v>660</v>
+        <v>680</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="M47" s="1"/>
+        <v>302</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>681</v>
+      </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="2">
-        <v>38.065479000000003</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>-97.345708000000002</v>
-      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="4"/>
-      <c r="T47" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="V47" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="AA47" t="s">
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>27</v>
-      </c>
-      <c r="AB47" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC47" t="s">
-        <v>388</v>
-      </c>
-      <c r="AE47" t="s">
-        <v>389</v>
-      </c>
-      <c r="AF47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG47" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>286</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="D48" t="s">
+        <v>173</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48">
+        <v>67117</v>
+      </c>
+      <c r="I48" t="s">
+        <v>174</v>
+      </c>
+      <c r="J48" t="s">
+        <v>84</v>
       </c>
       <c r="K48">
-        <v>682</v>
+        <v>660</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="M48" s="1"/>
-      <c r="N48" s="1" t="s">
-        <v>337</v>
-      </c>
+      <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
+      <c r="P48" s="2">
+        <v>38.065479000000003</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>-97.345708000000002</v>
+      </c>
       <c r="R48" s="2"/>
       <c r="S48" s="4"/>
       <c r="T48" s="1" t="s">
         <v>688</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>746</v>
+        <v>688</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
+        <v>745</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>388</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>389</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>286</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -6282,78 +6314,34 @@
       <c r="C49" t="s">
         <v>114</v>
       </c>
-      <c r="D49" t="s">
-        <v>175</v>
-      </c>
-      <c r="F49" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" t="s">
-        <v>82</v>
-      </c>
-      <c r="H49">
-        <v>66521</v>
-      </c>
-      <c r="I49" t="s">
-        <v>176</v>
-      </c>
-      <c r="J49" t="s">
-        <v>100</v>
-      </c>
       <c r="K49">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>682</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="M49" s="1"/>
       <c r="N49" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="P49" s="2">
-        <v>39.480414099999997</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>-96.177394699999994</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="O49" s="1"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
       <c r="S49" s="4"/>
       <c r="T49" s="1" t="s">
-        <v>747</v>
+        <v>688</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="AA49" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>28</v>
-      </c>
-      <c r="AB49" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC49" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE49" t="s">
-        <v>260</v>
-      </c>
-      <c r="AF49" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG49" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>29</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -6362,560 +6350,560 @@
         <v>114</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G50" t="s">
         <v>82</v>
       </c>
       <c r="H50">
-        <v>66866</v>
+        <v>66521</v>
       </c>
       <c r="I50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J50" t="s">
         <v>100</v>
       </c>
       <c r="K50">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>671</v>
+        <v>682</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P50" s="2">
-        <v>38.164371600000003</v>
+        <v>39.480414099999997</v>
       </c>
       <c r="Q50" s="2">
-        <v>-97.103965099999996</v>
+        <v>-96.177394699999994</v>
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="4"/>
       <c r="T50" s="1" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="AA50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB50" t="s">
         <v>339</v>
       </c>
       <c r="AC50" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AE50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF50" t="s">
         <v>82</v>
       </c>
       <c r="AG50" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>319</v>
+        <v>29</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
         <v>114</v>
       </c>
+      <c r="D51" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51">
+        <v>66866</v>
+      </c>
+      <c r="I51" t="s">
+        <v>178</v>
+      </c>
+      <c r="J51" t="s">
+        <v>100</v>
+      </c>
       <c r="K51">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>320</v>
+        <v>232</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
+        <v>261</v>
+      </c>
+      <c r="P51" s="2">
+        <v>38.164371600000003</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>-97.103965099999996</v>
+      </c>
       <c r="R51" s="2"/>
       <c r="S51" s="4"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T51" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>393</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="s">
         <v>114</v>
       </c>
-      <c r="D52" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" t="s">
-        <v>132</v>
-      </c>
-      <c r="G52" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52">
-        <v>67546</v>
-      </c>
-      <c r="I52" t="s">
-        <v>133</v>
-      </c>
-      <c r="J52" t="s">
-        <v>314</v>
-      </c>
       <c r="K52">
-        <v>50</v>
+        <v>720</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="M52" s="1"/>
+        <v>320</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="N52" s="1" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="P52" s="2">
-        <v>38.289691599999998</v>
-      </c>
-      <c r="Q52" s="2">
-        <v>-97.779943399999993</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="V52" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
         <v>114</v>
       </c>
+      <c r="D53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" t="s">
+        <v>132</v>
+      </c>
+      <c r="G53" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53">
+        <v>67546</v>
+      </c>
+      <c r="I53" t="s">
+        <v>133</v>
+      </c>
+      <c r="J53" t="s">
+        <v>314</v>
+      </c>
       <c r="K53">
-        <v>740</v>
+        <v>50</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
+      <c r="N53" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="P53" s="2">
+        <v>38.289691599999998</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>-97.779943399999993</v>
+      </c>
       <c r="R53" s="2"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T53" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>321</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
         <v>114</v>
       </c>
-      <c r="D54" t="s">
-        <v>180</v>
-      </c>
-      <c r="F54" t="s">
-        <v>181</v>
-      </c>
-      <c r="G54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H54">
-        <v>67579</v>
-      </c>
-      <c r="I54" t="s">
-        <v>182</v>
-      </c>
-      <c r="J54" t="s">
-        <v>183</v>
-      </c>
       <c r="K54">
-        <v>60</v>
+        <v>740</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>329</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
       <c r="O54" s="1"/>
-      <c r="P54" s="2">
-        <v>38.266167000000003</v>
-      </c>
-      <c r="Q54" s="2">
-        <v>-98.200824999999995</v>
-      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
       <c r="S54" s="4"/>
-      <c r="T54" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="V54" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="AA54" t="s">
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>179</v>
-      </c>
-      <c r="AB54" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC54" t="s">
-        <v>395</v>
-      </c>
-      <c r="AE54" t="s">
-        <v>396</v>
-      </c>
-      <c r="AF54" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG54" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>184</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D55" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F55" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G55" t="s">
         <v>82</v>
       </c>
       <c r="H55">
-        <v>67476</v>
+        <v>67579</v>
       </c>
       <c r="I55" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J55" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="K55">
-        <v>760</v>
+        <v>60</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>304</v>
+        <v>236</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="N55" s="1"/>
+        <v>683</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="O55" s="1"/>
       <c r="P55" s="2">
-        <v>38.551245999999999</v>
+        <v>38.266167000000003</v>
       </c>
       <c r="Q55" s="2">
-        <v>-97.429237000000001</v>
+        <v>-98.200824999999995</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="4"/>
       <c r="T55" s="1" t="s">
-        <v>754</v>
+        <v>688</v>
       </c>
       <c r="U55" s="1" t="s">
         <v>688</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+        <v>753</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>395</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>396</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G56" t="s">
         <v>82</v>
       </c>
       <c r="H56">
-        <v>67401</v>
+        <v>67476</v>
+      </c>
+      <c r="I56" t="s">
+        <v>186</v>
       </c>
       <c r="J56" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="K56">
-        <v>780</v>
+        <v>760</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1" t="s">
-        <v>262</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="2">
-        <v>38.855463999999998</v>
+        <v>38.551245999999999</v>
       </c>
       <c r="Q56" s="2">
-        <v>-97.614002999999997</v>
+        <v>-97.429237000000001</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="4"/>
       <c r="T56" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="U56" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="U56" s="1" t="s">
-        <v>756</v>
-      </c>
       <c r="V56" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="AA56" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>187</v>
-      </c>
-      <c r="AB56" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC56" t="s">
-        <v>398</v>
-      </c>
-      <c r="AE56" t="s">
-        <v>262</v>
-      </c>
-      <c r="AF56" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG56" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>30</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="G57" t="s">
         <v>82</v>
       </c>
       <c r="H57">
-        <v>67480</v>
-      </c>
-      <c r="I57" t="s">
-        <v>190</v>
+        <v>67401</v>
       </c>
       <c r="J57" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="K57">
-        <v>800</v>
+        <v>780</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>672</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="M57" s="1"/>
       <c r="N57" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>263</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="O57" s="1"/>
       <c r="P57" s="2">
-        <v>38.917464000000002</v>
+        <v>38.855463999999998</v>
       </c>
       <c r="Q57" s="2">
-        <v>-97.374758999999997</v>
+        <v>-97.614002999999997</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="4"/>
       <c r="T57" s="1" t="s">
-        <v>757</v>
+        <v>688</v>
       </c>
       <c r="U57" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="V57" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="V57" s="1" t="s">
-        <v>758</v>
-      </c>
       <c r="AA57" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="AB57" t="s">
         <v>339</v>
       </c>
       <c r="AC57" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AE57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AF57" t="s">
         <v>82</v>
       </c>
       <c r="AG57" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G58" t="s">
         <v>82</v>
       </c>
       <c r="H58">
-        <v>67482</v>
+        <v>67480</v>
       </c>
       <c r="I58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J58" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="K58">
-        <v>820</v>
+        <v>800</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P58" s="2">
-        <v>39.026199400000003</v>
+        <v>38.917464000000002</v>
       </c>
       <c r="Q58" s="2">
-        <v>-97.259965699999995</v>
+        <v>-97.374758999999997</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="4"/>
       <c r="T58" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>760</v>
+        <v>688</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="AA58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB58" t="s">
         <v>339</v>
       </c>
       <c r="AC58" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AE58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF58" t="s">
         <v>82</v>
       </c>
       <c r="AG58" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>309</v>
+        <v>31</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -6923,26 +6911,78 @@
       <c r="C59" t="s">
         <v>114</v>
       </c>
+      <c r="D59" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" t="s">
+        <v>82</v>
+      </c>
+      <c r="H59">
+        <v>67482</v>
+      </c>
+      <c r="I59" t="s">
+        <v>192</v>
+      </c>
+      <c r="J59" t="s">
+        <v>100</v>
+      </c>
       <c r="K59">
-        <v>18</v>
+        <v>820</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="P59" s="2">
+        <v>39.026199400000003</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>-97.259965699999995</v>
+      </c>
       <c r="R59" s="2"/>
       <c r="S59" s="4"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="1"/>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T59" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>402</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>264</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>309</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -6950,78 +6990,26 @@
       <c r="C60" t="s">
         <v>114</v>
       </c>
-      <c r="D60" t="s">
-        <v>193</v>
-      </c>
-      <c r="F60" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" t="s">
-        <v>82</v>
-      </c>
-      <c r="H60">
-        <v>67151</v>
-      </c>
-      <c r="I60" t="s">
-        <v>194</v>
-      </c>
-      <c r="J60" t="s">
-        <v>100</v>
-      </c>
       <c r="K60">
-        <v>840</v>
+        <v>18</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="P60" s="2">
-        <v>38.218391099999998</v>
-      </c>
-      <c r="Q60" s="2">
-        <v>-97.229442399999996</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
       <c r="S60" s="4"/>
-      <c r="T60" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="V60" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="AA60" t="s">
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>32</v>
-      </c>
-      <c r="AB60" t="s">
-        <v>339</v>
-      </c>
-      <c r="AC60" t="s">
-        <v>404</v>
-      </c>
-      <c r="AE60" t="s">
-        <v>265</v>
-      </c>
-      <c r="AF60" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG60">
-        <v>67151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>33</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -7030,73 +7018,77 @@
         <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G61" t="s">
         <v>82</v>
       </c>
       <c r="H61">
-        <v>66549</v>
+        <v>67151</v>
       </c>
       <c r="I61" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J61" t="s">
-        <v>770</v>
+        <v>100</v>
       </c>
       <c r="K61">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="M61" s="1"/>
+        <v>237</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="N61" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="O61" s="1"/>
+        <v>265</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="P61" s="2">
-        <v>39.3915431</v>
+        <v>38.218391099999998</v>
       </c>
       <c r="Q61" s="2">
-        <v>-96.410154700000007</v>
+        <v>-97.229442399999996</v>
       </c>
       <c r="R61" s="2"/>
       <c r="S61" s="4"/>
       <c r="T61" s="1" t="s">
-        <v>659</v>
+        <v>762</v>
       </c>
       <c r="U61" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>688</v>
+        <v>764</v>
       </c>
       <c r="AA61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB61" t="s">
         <v>339</v>
       </c>
       <c r="AC61" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AE61" t="s">
-        <v>406</v>
+        <v>265</v>
       </c>
       <c r="AF61" t="s">
         <v>82</v>
       </c>
-      <c r="AG61" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG61">
+        <v>67151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -7105,150 +7097,152 @@
         <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F62" t="s">
-        <v>197</v>
+        <v>33</v>
       </c>
       <c r="G62" t="s">
         <v>82</v>
       </c>
       <c r="H62">
-        <v>67154</v>
+        <v>66549</v>
       </c>
       <c r="I62" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J62" t="s">
-        <v>94</v>
+        <v>770</v>
       </c>
       <c r="K62">
-        <v>860</v>
+        <v>845</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>654</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="M62" s="1"/>
       <c r="N62" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>429</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="O62" s="1"/>
       <c r="P62" s="2">
-        <v>37.962503599999998</v>
+        <v>39.3915431</v>
       </c>
       <c r="Q62" s="2">
-        <v>-97.150157199999995</v>
+        <v>-96.410154700000007</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="4"/>
       <c r="T62" s="1" t="s">
-        <v>766</v>
+        <v>659</v>
       </c>
       <c r="U62" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="V62" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="V62" s="1" t="s">
-        <v>767</v>
-      </c>
       <c r="AA62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB62" t="s">
         <v>339</v>
       </c>
       <c r="AC62" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="AE62" t="s">
-        <v>266</v>
+        <v>406</v>
       </c>
       <c r="AF62" t="s">
         <v>82</v>
       </c>
-      <c r="AG62">
-        <v>67154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG62" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F63" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G63" t="s">
         <v>82</v>
       </c>
       <c r="H63">
-        <v>67201</v>
+        <v>67154</v>
       </c>
       <c r="I63" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J63" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K63">
-        <v>880</v>
+        <v>860</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
+        <v>239</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="P63" s="2">
-        <v>37.739190899999997</v>
+        <v>37.962503599999998</v>
       </c>
       <c r="Q63" s="2">
-        <v>-97.329066100000006</v>
+        <v>-97.150157199999995</v>
       </c>
       <c r="R63" s="2"/>
       <c r="S63" s="4"/>
       <c r="T63" s="1" t="s">
-        <v>688</v>
+        <v>766</v>
       </c>
       <c r="U63" s="1" t="s">
         <v>688</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AA63" t="s">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="AB63" t="s">
         <v>339</v>
       </c>
       <c r="AC63" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AE63" t="s">
-        <v>410</v>
+        <v>266</v>
       </c>
       <c r="AF63" t="s">
         <v>82</v>
       </c>
-      <c r="AG63" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG63">
+        <v>67154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -7257,39 +7251,37 @@
         <v>115</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F64" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
       <c r="G64" t="s">
         <v>82</v>
       </c>
       <c r="H64">
-        <v>67491</v>
+        <v>67201</v>
       </c>
       <c r="I64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J64" t="s">
         <v>84</v>
       </c>
       <c r="K64">
-        <v>900</v>
+        <v>880</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>684</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="2">
-        <v>38.385244999999998</v>
+        <v>37.739190899999997</v>
       </c>
       <c r="Q64" s="2">
-        <v>-97.909503999999998</v>
+        <v>-97.329066100000006</v>
       </c>
       <c r="R64" s="2"/>
       <c r="S64" s="4"/>
@@ -7300,24 +7292,99 @@
         <v>688</v>
       </c>
       <c r="V64" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AA64" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="AB64" t="s">
         <v>339</v>
       </c>
       <c r="AC64" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="AE64" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="AF64" t="s">
         <v>82</v>
       </c>
       <c r="AG64" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" t="s">
+        <v>82</v>
+      </c>
+      <c r="H65">
+        <v>67491</v>
+      </c>
+      <c r="I65" t="s">
+        <v>205</v>
+      </c>
+      <c r="J65" t="s">
+        <v>84</v>
+      </c>
+      <c r="K65">
+        <v>900</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="2">
+        <v>38.385244999999998</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>-97.909503999999998</v>
+      </c>
+      <c r="R65" s="2"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="V65" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>412</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>413</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG65" t="s">
         <v>414</v>
       </c>
     </row>
@@ -7343,21 +7410,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>640</v>
       </c>
@@ -7398,7 +7465,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -7427,7 +7494,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
@@ -7440,7 +7507,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>21</v>
       </c>
@@ -7466,7 +7533,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31</v>
       </c>
@@ -7495,7 +7562,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>32</v>
       </c>
@@ -7514,7 +7581,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>41</v>
       </c>
@@ -7531,7 +7598,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>61</v>
       </c>
@@ -7560,7 +7627,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>71</v>
       </c>
@@ -7592,7 +7659,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>81</v>
       </c>
@@ -7615,7 +7682,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>91</v>
       </c>
@@ -7641,7 +7708,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>101</v>
       </c>
@@ -7664,7 +7731,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>111</v>
       </c>
@@ -7690,7 +7757,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>121</v>
       </c>
@@ -7716,7 +7783,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>131</v>
       </c>
@@ -7745,7 +7812,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>141</v>
       </c>
@@ -7768,7 +7835,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>151</v>
       </c>
@@ -7794,7 +7861,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>161</v>
       </c>
@@ -7817,7 +7884,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>171</v>
       </c>
@@ -7843,7 +7910,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>181</v>
       </c>
@@ -7863,7 +7930,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>182</v>
       </c>
@@ -7881,7 +7948,7 @@
       <c r="H21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>183</v>
       </c>
@@ -7907,7 +7974,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>185</v>
       </c>
@@ -7924,7 +7991,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>187</v>
       </c>
@@ -7947,7 +8014,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>188</v>
       </c>
@@ -7964,7 +8031,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>190</v>
       </c>
@@ -7982,7 +8049,7 @@
       <c r="H26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>191</v>
       </c>
@@ -8008,7 +8075,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>192</v>
       </c>
@@ -8037,7 +8104,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>193</v>
       </c>
@@ -8063,7 +8130,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>194</v>
       </c>
@@ -8089,7 +8156,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>195</v>
       </c>
@@ -8115,7 +8182,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>196</v>
       </c>
@@ -8141,7 +8208,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>197</v>
       </c>
@@ -8159,7 +8226,7 @@
       <c r="H33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>198</v>
       </c>
@@ -8182,7 +8249,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>199</v>
       </c>
@@ -8200,7 +8267,7 @@
       <c r="H35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>201</v>
       </c>
@@ -8211,7 +8278,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>205</v>
       </c>
@@ -8234,7 +8301,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>212</v>
       </c>
@@ -8263,7 +8330,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>215</v>
       </c>
@@ -8282,7 +8349,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>222</v>
       </c>
@@ -8308,7 +8375,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>242</v>
       </c>
@@ -8334,7 +8401,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>245</v>
       </c>
@@ -8352,7 +8419,7 @@
       <c r="H42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>252</v>
       </c>
@@ -8378,7 +8445,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>262</v>
       </c>
@@ -8404,7 +8471,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>272</v>
       </c>
@@ -8430,7 +8497,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>282</v>
       </c>
@@ -8448,7 +8515,7 @@
       <c r="H46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>291</v>
       </c>
@@ -8466,7 +8533,7 @@
       <c r="H47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>292</v>
       </c>
@@ -8492,7 +8559,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>293</v>
       </c>
@@ -8515,7 +8582,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>294</v>
       </c>
@@ -8538,7 +8605,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>295</v>
       </c>
@@ -8561,7 +8628,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>296</v>
       </c>
@@ -8578,7 +8645,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>311</v>
       </c>
@@ -8610,7 +8677,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>315</v>
       </c>
@@ -8630,7 +8697,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>331</v>
       </c>
@@ -8656,7 +8723,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>341</v>
       </c>
@@ -8682,7 +8749,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>351</v>
       </c>
@@ -8708,7 +8775,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>361</v>
       </c>
@@ -8729,7 +8796,7 @@
       </c>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>432</v>
       </c>
@@ -8746,7 +8813,7 @@
       <c r="G59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>433</v>
       </c>
@@ -8772,7 +8839,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>442</v>
       </c>
@@ -8798,7 +8865,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>443</v>
       </c>
@@ -8824,7 +8891,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>445</v>
       </c>
@@ -8842,7 +8909,7 @@
       <c r="H63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>447</v>
       </c>
@@ -8865,7 +8932,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>510</v>
       </c>
@@ -8891,7 +8958,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>520</v>
       </c>
@@ -8917,7 +8984,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>530</v>
       </c>
@@ -8943,7 +9010,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>540</v>
       </c>
@@ -8969,7 +9036,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>541</v>
       </c>
@@ -8992,7 +9059,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>542</v>
       </c>
@@ -9018,7 +9085,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>543</v>
       </c>
@@ -9044,7 +9111,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>544</v>
       </c>
@@ -9070,7 +9137,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>545</v>
       </c>
@@ -9093,7 +9160,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>546</v>
       </c>
@@ -9119,7 +9186,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>547</v>
       </c>
@@ -9145,7 +9212,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>548</v>
       </c>
@@ -9171,7 +9238,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>549</v>
       </c>
@@ -9194,7 +9261,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>550</v>
       </c>
@@ -9217,7 +9284,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>551</v>
       </c>
@@ -9243,7 +9310,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>560</v>
       </c>
@@ -9261,7 +9328,7 @@
       <c r="H80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>561</v>
       </c>
@@ -9284,7 +9351,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>570</v>
       </c>
@@ -9301,7 +9368,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>571</v>
       </c>
@@ -9316,7 +9383,7 @@
       </c>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>630</v>
       </c>
@@ -9339,7 +9406,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>632</v>
       </c>
@@ -9362,7 +9429,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>634</v>
       </c>
@@ -9382,7 +9449,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>636</v>
       </c>
@@ -9405,7 +9472,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>642</v>
       </c>
@@ -9428,7 +9495,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>644</v>
       </c>
@@ -9451,7 +9518,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>646</v>
       </c>
@@ -9474,7 +9541,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>650</v>
       </c>
@@ -9497,7 +9564,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>940</v>
       </c>

</xml_diff>

<commit_message>
Additional location update for new GP GL 035 location Manhattan Bulk Fuel in the spreadsheet
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="822">
   <si>
     <t>Abilene</t>
   </si>
@@ -2483,9 +2483,6 @@
   </si>
   <si>
     <t>Manhattan Bulk Fuel</t>
-  </si>
-  <si>
-    <t>3384 Excel Rd</t>
   </si>
   <si>
     <t>Bulk fuel and oil</t>
@@ -3178,7 +3175,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
@@ -5495,7 +5492,7 @@
         <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>819</v>
+        <v>151</v>
       </c>
       <c r="F35" t="s">
         <v>23</v>
@@ -5506,8 +5503,11 @@
       <c r="H35">
         <v>66502</v>
       </c>
+      <c r="I35" t="s">
+        <v>149</v>
+      </c>
       <c r="J35" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K35">
         <v>34</v>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="2"/>

</xml_diff>

<commit_message>
add MWF location and Sumner Co
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="830">
   <si>
     <t>Abilene</t>
   </si>
@@ -2492,6 +2492,30 @@
   </si>
   <si>
     <t>Manhattan Builk Fuel</t>
+  </si>
+  <si>
+    <t>DEERFIELD</t>
+  </si>
+  <si>
+    <t>SUMNER CO TERMINAL</t>
+  </si>
+  <si>
+    <t>Deerfield</t>
+  </si>
+  <si>
+    <t>201 S. Walnut</t>
+  </si>
+  <si>
+    <t>(417) 966-7303</t>
+  </si>
+  <si>
+    <t>(417) 966-7302</t>
+  </si>
+  <si>
+    <t>Sumner Co. Terminal</t>
+  </si>
+  <si>
+    <t>1063 W. 10th Ave.</t>
   </si>
 </sst>
 </file>
@@ -2638,8 +2662,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M92" totalsRowShown="0">
-  <autoFilter ref="A1:M92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M94" totalsRowShown="0">
+  <autoFilter ref="A1:M94"/>
   <sortState ref="A2:M92">
     <sortCondition ref="A2:A92"/>
   </sortState>
@@ -2966,14 +2990,14 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2981,7 +3005,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2989,7 +3013,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2997,7 +3021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3005,7 +3029,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3013,7 +3037,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3021,7 +3045,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3029,7 +3053,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3037,7 +3061,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3045,7 +3069,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3053,7 +3077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3061,7 +3085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -3069,7 +3093,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3077,7 +3101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3085,7 +3109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3093,7 +3117,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3101,7 +3125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3109,7 +3133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3117,7 +3141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3125,7 +3149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3133,7 +3157,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3141,7 +3165,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3149,7 +3173,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3157,7 +3181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3165,7 +3189,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>821</v>
       </c>
@@ -3181,7 +3205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -3189,7 +3213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3197,7 +3221,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3205,17 +3229,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3223,7 +3247,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3231,7 +3255,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -3239,7 +3263,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>172</v>
       </c>
@@ -3247,7 +3271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -3255,7 +3279,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -3263,7 +3287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -3271,7 +3295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>314</v>
       </c>
@@ -3279,7 +3303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -3287,7 +3311,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>184</v>
       </c>
@@ -3295,7 +3319,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>187</v>
       </c>
@@ -3303,7 +3327,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -3311,7 +3335,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3319,7 +3343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -3327,7 +3351,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3335,7 +3359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -3343,7 +3367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>200</v>
       </c>
@@ -3351,7 +3375,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -3374,36 +3398,36 @@
   </sheetPr>
   <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="40.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="15" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="40.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="15" width="14.5546875" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3474,7 +3498,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3553,7 +3577,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3614,7 +3638,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3689,7 +3713,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3768,7 +3792,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3847,7 +3871,7 @@
         <v>67017</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3904,7 +3928,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3983,7 +4007,7 @@
         <v>67522</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>288</v>
       </c>
@@ -4018,7 +4042,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4097,7 +4121,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -4166,7 +4190,7 @@
         <v>67428</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4245,7 +4269,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -4274,7 +4298,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>281</v>
       </c>
@@ -4317,7 +4341,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4388,7 +4412,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4465,7 +4489,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -4496,7 +4520,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4553,7 +4577,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4632,7 +4656,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4693,7 +4717,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4754,7 +4778,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -4833,7 +4857,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -4912,7 +4936,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -4943,7 +4967,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -5018,7 +5042,7 @@
         <v>67443</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -5069,7 +5093,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>316</v>
       </c>
@@ -5100,7 +5124,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -5129,7 +5153,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5204,7 +5228,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -5283,7 +5307,7 @@
         <v>67456</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -5344,7 +5368,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>284</v>
       </c>
@@ -5377,7 +5401,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -5406,7 +5430,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -5481,7 +5505,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>818</v>
       </c>
@@ -5528,7 +5552,7 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>150</v>
       </c>
@@ -5607,7 +5631,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -5686,7 +5710,7 @@
         <v>67464</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>336</v>
       </c>
@@ -5719,7 +5743,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -5770,7 +5794,7 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -5830,7 +5854,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -5890,7 +5914,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>287</v>
       </c>
@@ -5919,7 +5943,7 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -5996,7 +6020,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -6062,7 +6086,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -6144,7 +6168,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -6202,7 +6226,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>285</v>
       </c>
@@ -6231,7 +6255,7 @@
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -6304,7 +6328,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>286</v>
       </c>
@@ -6339,7 +6363,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -6418,7 +6442,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -6497,7 +6521,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>319</v>
       </c>
@@ -6530,7 +6554,7 @@
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>314</v>
       </c>
@@ -6589,7 +6613,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>321</v>
       </c>
@@ -6616,7 +6640,7 @@
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -6693,7 +6717,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>184</v>
       </c>
@@ -6750,7 +6774,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -6822,7 +6846,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -6901,7 +6925,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -6980,7 +7004,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>309</v>
       </c>
@@ -7007,7 +7031,7 @@
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -7086,7 +7110,7 @@
         <v>67151</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -7161,7 +7185,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -7240,7 +7264,7 @@
         <v>67154</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>200</v>
       </c>
@@ -7313,7 +7337,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -7403,28 +7427,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>640</v>
       </c>
@@ -7465,7 +7489,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11</v>
       </c>
@@ -7494,7 +7518,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>13</v>
       </c>
@@ -7507,7 +7531,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>21</v>
       </c>
@@ -7533,7 +7557,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>31</v>
       </c>
@@ -7562,7 +7586,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>32</v>
       </c>
@@ -7581,7 +7605,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>41</v>
       </c>
@@ -7598,7 +7622,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>61</v>
       </c>
@@ -7627,7 +7651,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>71</v>
       </c>
@@ -7659,7 +7683,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>81</v>
       </c>
@@ -7682,7 +7706,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>91</v>
       </c>
@@ -7708,7 +7732,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>101</v>
       </c>
@@ -7731,7 +7755,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>111</v>
       </c>
@@ -7757,7 +7781,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>121</v>
       </c>
@@ -7783,7 +7807,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>131</v>
       </c>
@@ -7812,7 +7836,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>141</v>
       </c>
@@ -7835,7 +7859,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>151</v>
       </c>
@@ -7861,7 +7885,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>161</v>
       </c>
@@ -7884,7 +7908,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>171</v>
       </c>
@@ -7910,7 +7934,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>181</v>
       </c>
@@ -7930,7 +7954,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>182</v>
       </c>
@@ -7948,7 +7972,7 @@
       <c r="H21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>183</v>
       </c>
@@ -7974,7 +7998,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>185</v>
       </c>
@@ -7991,7 +8015,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>187</v>
       </c>
@@ -8014,7 +8038,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>188</v>
       </c>
@@ -8031,7 +8055,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>190</v>
       </c>
@@ -8049,7 +8073,7 @@
       <c r="H26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>191</v>
       </c>
@@ -8075,7 +8099,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>192</v>
       </c>
@@ -8104,7 +8128,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>193</v>
       </c>
@@ -8130,7 +8154,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>194</v>
       </c>
@@ -8156,7 +8180,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>195</v>
       </c>
@@ -8182,7 +8206,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>196</v>
       </c>
@@ -8208,7 +8232,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>197</v>
       </c>
@@ -8226,7 +8250,7 @@
       <c r="H33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>198</v>
       </c>
@@ -8249,7 +8273,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>199</v>
       </c>
@@ -8267,7 +8291,7 @@
       <c r="H35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>201</v>
       </c>
@@ -8278,7 +8302,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>205</v>
       </c>
@@ -8301,7 +8325,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>212</v>
       </c>
@@ -8330,7 +8354,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>215</v>
       </c>
@@ -8349,7 +8373,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>222</v>
       </c>
@@ -8375,7 +8399,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>242</v>
       </c>
@@ -8401,7 +8425,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>245</v>
       </c>
@@ -8419,7 +8443,7 @@
       <c r="H42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>252</v>
       </c>
@@ -8445,7 +8469,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>262</v>
       </c>
@@ -8471,7 +8495,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>272</v>
       </c>
@@ -8497,7 +8521,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>282</v>
       </c>
@@ -8515,7 +8539,7 @@
       <c r="H46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>291</v>
       </c>
@@ -8533,7 +8557,7 @@
       <c r="H47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>292</v>
       </c>
@@ -8559,7 +8583,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>293</v>
       </c>
@@ -8582,7 +8606,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>294</v>
       </c>
@@ -8605,7 +8629,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>295</v>
       </c>
@@ -8628,7 +8652,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>296</v>
       </c>
@@ -8645,7 +8669,7 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>311</v>
       </c>
@@ -8677,7 +8701,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>315</v>
       </c>
@@ -8697,7 +8721,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>331</v>
       </c>
@@ -8723,7 +8747,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>341</v>
       </c>
@@ -8749,7 +8773,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>351</v>
       </c>
@@ -8775,7 +8799,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>361</v>
       </c>
@@ -8796,7 +8820,7 @@
       </c>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>432</v>
       </c>
@@ -8813,7 +8837,7 @@
       <c r="G59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>433</v>
       </c>
@@ -8839,7 +8863,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>442</v>
       </c>
@@ -8865,7 +8889,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>443</v>
       </c>
@@ -8891,7 +8915,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>445</v>
       </c>
@@ -8909,7 +8933,7 @@
       <c r="H63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>447</v>
       </c>
@@ -8932,7 +8956,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>510</v>
       </c>
@@ -8958,7 +8982,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>520</v>
       </c>
@@ -8984,7 +9008,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>530</v>
       </c>
@@ -9010,7 +9034,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>540</v>
       </c>
@@ -9036,7 +9060,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>541</v>
       </c>
@@ -9059,7 +9083,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>542</v>
       </c>
@@ -9085,7 +9109,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>543</v>
       </c>
@@ -9111,7 +9135,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>544</v>
       </c>
@@ -9137,7 +9161,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>545</v>
       </c>
@@ -9160,7 +9184,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>546</v>
       </c>
@@ -9186,7 +9210,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>547</v>
       </c>
@@ -9212,7 +9236,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>548</v>
       </c>
@@ -9238,7 +9262,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>549</v>
       </c>
@@ -9261,7 +9285,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>550</v>
       </c>
@@ -9284,7 +9308,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>551</v>
       </c>
@@ -9310,7 +9334,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>560</v>
       </c>
@@ -9328,7 +9352,7 @@
       <c r="H80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>561</v>
       </c>
@@ -9351,229 +9375,267 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
+        <v>562</v>
+      </c>
+      <c r="B82" t="s">
+        <v>823</v>
+      </c>
+      <c r="D82" t="s">
+        <v>644</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83">
         <v>570</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>436</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="F83" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H83" s="3" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84">
         <v>571</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>643</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="H83" s="3"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85">
         <v>630</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>778</v>
-      </c>
-      <c r="D84" t="s">
-        <v>786</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>795</v>
-      </c>
-      <c r="H84" t="s">
-        <v>796</v>
-      </c>
-      <c r="K84" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>632</v>
-      </c>
-      <c r="B85" t="s">
-        <v>779</v>
       </c>
       <c r="D85" t="s">
         <v>786</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>798</v>
+        <v>795</v>
+      </c>
+      <c r="H85" t="s">
+        <v>796</v>
       </c>
       <c r="K85" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B86" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D86" t="s">
         <v>786</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+        <v>798</v>
+      </c>
+      <c r="K86" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B87" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D87" t="s">
         <v>786</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="K87" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B88" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D88" t="s">
         <v>786</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="K88" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B89" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D89" t="s">
         <v>786</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="K89" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="B90" t="s">
-        <v>784</v>
+        <v>822</v>
       </c>
       <c r="D90" t="s">
         <v>786</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>793</v>
+        <v>824</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>812</v>
+        <v>825</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>813</v>
+        <v>826</v>
       </c>
       <c r="K90" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B91" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D91" t="s">
         <v>786</v>
       </c>
       <c r="F91" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="K91" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>646</v>
+      </c>
+      <c r="B92" t="s">
+        <v>784</v>
+      </c>
+      <c r="D92" t="s">
+        <v>786</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="K92" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>650</v>
+      </c>
+      <c r="B93" t="s">
+        <v>785</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>794</v>
       </c>
-      <c r="G91" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>815</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="H93" s="3" t="s">
         <v>816</v>
       </c>
-      <c r="K91" t="s">
+      <c r="K93" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94">
         <v>940</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>642</v>
       </c>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
New TMA Locations: Sumner County, Deerfield
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="831">
   <si>
     <t>Abilene</t>
   </si>
@@ -2492,6 +2492,33 @@
   </si>
   <si>
     <t>Manhattan Builk Fuel</t>
+  </si>
+  <si>
+    <t>SUMNER COUNTY</t>
+  </si>
+  <si>
+    <t>Sumner County Terminal</t>
+  </si>
+  <si>
+    <t>1063 W 10th Ave</t>
+  </si>
+  <si>
+    <t>(620) 747-9136</t>
+  </si>
+  <si>
+    <t>DEERFIELD</t>
+  </si>
+  <si>
+    <t>Deerfield</t>
+  </si>
+  <si>
+    <t>201 S Walnut</t>
+  </si>
+  <si>
+    <t>(417) 966-7303</t>
+  </si>
+  <si>
+    <t>(417) 966-7302</t>
   </si>
 </sst>
 </file>
@@ -2638,8 +2665,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M92" totalsRowShown="0">
-  <autoFilter ref="A1:M92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M94" totalsRowShown="0">
+  <autoFilter ref="A1:M94"/>
   <sortState ref="A2:M92">
     <sortCondition ref="A2:A92"/>
   </sortState>
@@ -7403,7 +7430,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9353,227 +9380,270 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="B82" t="s">
-        <v>436</v>
+        <v>822</v>
+      </c>
+      <c r="D82" t="s">
+        <v>644</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>435</v>
+        <v>823</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>434</v>
+        <v>824</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>433</v>
+        <v>825</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B83" t="s">
-        <v>643</v>
+        <v>436</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="H83" s="3"/>
+        <v>434</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>630</v>
+        <v>571</v>
       </c>
       <c r="B84" t="s">
-        <v>778</v>
-      </c>
-      <c r="D84" t="s">
-        <v>786</v>
+        <v>643</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>787</v>
+        <v>432</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>795</v>
-      </c>
-      <c r="H84" t="s">
-        <v>796</v>
-      </c>
-      <c r="K84" t="s">
-        <v>797</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B85" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D85" t="s">
         <v>786</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>798</v>
+        <v>795</v>
+      </c>
+      <c r="H85" t="s">
+        <v>796</v>
       </c>
       <c r="K85" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B86" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D86" t="s">
         <v>786</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>802</v>
+        <v>798</v>
+      </c>
+      <c r="K86" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B87" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D87" t="s">
         <v>786</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="K87" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B88" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D88" t="s">
         <v>786</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="K88" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B89" t="s">
-        <v>783</v>
+        <v>826</v>
       </c>
       <c r="D89" t="s">
         <v>786</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>792</v>
+        <v>827</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>809</v>
+        <v>828</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>810</v>
+        <v>829</v>
       </c>
       <c r="K89" t="s">
-        <v>811</v>
+        <v>830</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B90" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D90" t="s">
         <v>786</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="K90" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B91" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D91" t="s">
         <v>786</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="K91" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
+        <v>646</v>
+      </c>
+      <c r="B92" t="s">
+        <v>784</v>
+      </c>
+      <c r="D92" t="s">
+        <v>786</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="K92" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>650</v>
+      </c>
+      <c r="B93" t="s">
+        <v>785</v>
+      </c>
+      <c r="D93" t="s">
+        <v>786</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="K93" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>940</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>642</v>
       </c>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
Added additional requested products to the Harvest Summary report
01 WHEAT
02 MILO
03 SOYBEANS
04 CORN
06 BARLEY*
22 SUNFLOWERS*
27 CANOLA
28 SOFT RED WHEAT*

ORDER ADDED: 01, 02, 03, 04, 27, 22, 06, 28
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -2990,14 +2990,14 @@
       <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>818</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3229,17 +3229,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>172</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>314</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>184</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>187</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>200</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -3402,32 +3402,32 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
-    <col min="14" max="15" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>67017</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>67522</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>288</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>67428</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -4298,7 +4298,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>281</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -4520,7 +4520,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -4967,7 +4967,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>67443</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -5093,7 +5093,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>316</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -5153,7 +5153,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>67456</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>284</v>
       </c>
@@ -5401,7 +5401,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -5430,7 +5430,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>818</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>150</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>67464</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>336</v>
       </c>
@@ -5743,7 +5743,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -5794,7 +5794,7 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>287</v>
       </c>
@@ -5943,7 +5943,7 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>285</v>
       </c>
@@ -6255,7 +6255,7 @@
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>286</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>319</v>
       </c>
@@ -6554,7 +6554,7 @@
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>314</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>321</v>
       </c>
@@ -6640,7 +6640,7 @@
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>184</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>309</v>
       </c>
@@ -7031,7 +7031,7 @@
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>67151</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>67154</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>200</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -7430,25 +7430,25 @@
   <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>640</v>
       </c>
@@ -7489,7 +7489,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
@@ -7531,7 +7531,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>21</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>32</v>
       </c>
@@ -7605,7 +7605,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>41</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>61</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>71</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>81</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>91</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>101</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>111</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>121</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>131</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>141</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>151</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>161</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>171</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>181</v>
       </c>
@@ -7954,7 +7954,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>182</v>
       </c>
@@ -7972,7 +7972,7 @@
       <c r="H21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>183</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>185</v>
       </c>
@@ -8015,7 +8015,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>187</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>188</v>
       </c>
@@ -8055,7 +8055,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>190</v>
       </c>
@@ -8073,7 +8073,7 @@
       <c r="H26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>191</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>192</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>193</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>194</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>195</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>196</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>197</v>
       </c>
@@ -8250,7 +8250,7 @@
       <c r="H33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>198</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>199</v>
       </c>
@@ -8291,7 +8291,7 @@
       <c r="H35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>200</v>
       </c>
@@ -8309,7 +8309,7 @@
       <c r="H36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>201</v>
       </c>
@@ -8320,7 +8320,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>205</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>212</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>215</v>
       </c>
@@ -8391,7 +8391,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>222</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>242</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>245</v>
       </c>
@@ -8461,7 +8461,7 @@
       <c r="H43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>252</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>262</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>272</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>282</v>
       </c>
@@ -8557,7 +8557,7 @@
       <c r="H47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>291</v>
       </c>
@@ -8575,7 +8575,7 @@
       <c r="H48" s="3"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>292</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>293</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>294</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>295</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>296</v>
       </c>
@@ -8687,7 +8687,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>311</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>315</v>
       </c>
@@ -8739,7 +8739,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>331</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>341</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>351</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>361</v>
       </c>
@@ -8838,7 +8838,7 @@
       </c>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>432</v>
       </c>
@@ -8855,7 +8855,7 @@
       <c r="G60" s="3"/>
       <c r="K60" s="3"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>433</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>442</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>443</v>
       </c>
@@ -8933,7 +8933,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>445</v>
       </c>
@@ -8951,7 +8951,7 @@
       <c r="H64" s="3"/>
       <c r="K64" s="3"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>447</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>510</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>520</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>530</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>540</v>
       </c>
@@ -9078,7 +9078,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>541</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>542</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>543</v>
       </c>
@@ -9153,7 +9153,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>544</v>
       </c>
@@ -9179,7 +9179,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>545</v>
       </c>
@@ -9202,7 +9202,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>546</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>547</v>
       </c>
@@ -9254,7 +9254,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>548</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>549</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>550</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>551</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>560</v>
       </c>
@@ -9370,7 +9370,7 @@
       <c r="H81" s="3"/>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>561</v>
       </c>
@@ -9393,7 +9393,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>562</v>
       </c>
@@ -9403,6 +9403,9 @@
       <c r="D83" t="s">
         <v>644</v>
       </c>
+      <c r="E83">
+        <v>6750000</v>
+      </c>
       <c r="F83" s="3" t="s">
         <v>827</v>
       </c>
@@ -9411,7 +9414,7 @@
       </c>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>570</v>
       </c>
@@ -9428,7 +9431,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>571</v>
       </c>
@@ -9443,7 +9446,7 @@
       </c>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>630</v>
       </c>
@@ -9466,7 +9469,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>632</v>
       </c>
@@ -9489,7 +9492,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>634</v>
       </c>
@@ -9509,7 +9512,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>636</v>
       </c>
@@ -9532,7 +9535,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>642</v>
       </c>
@@ -9555,7 +9558,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>640</v>
       </c>
@@ -9578,7 +9581,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>644</v>
       </c>
@@ -9601,7 +9604,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>646</v>
       </c>
@@ -9624,7 +9627,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>650</v>
       </c>
@@ -9644,7 +9647,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>940</v>
       </c>

</xml_diff>

<commit_message>
Updated Average calculation so arrows will display correctly as well as MWF missing 90% location capacities; sorting on percentage columns
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
@@ -9456,6 +9456,9 @@
       <c r="D86" t="s">
         <v>786</v>
       </c>
+      <c r="E86">
+        <v>457000</v>
+      </c>
       <c r="F86" s="3" t="s">
         <v>787</v>
       </c>
@@ -9479,6 +9482,9 @@
       <c r="D87" t="s">
         <v>786</v>
       </c>
+      <c r="E87">
+        <v>140310</v>
+      </c>
       <c r="F87" s="3" t="s">
         <v>788</v>
       </c>
@@ -9502,6 +9508,9 @@
       <c r="D88" t="s">
         <v>786</v>
       </c>
+      <c r="E88">
+        <v>249000</v>
+      </c>
       <c r="F88" s="3" t="s">
         <v>789</v>
       </c>
@@ -9522,6 +9531,9 @@
       <c r="D89" t="s">
         <v>786</v>
       </c>
+      <c r="E89">
+        <v>130000</v>
+      </c>
       <c r="F89" s="3" t="s">
         <v>790</v>
       </c>
@@ -9545,6 +9557,9 @@
       <c r="D90" t="s">
         <v>786</v>
       </c>
+      <c r="E90">
+        <v>247500</v>
+      </c>
       <c r="F90" s="3" t="s">
         <v>791</v>
       </c>
@@ -9568,6 +9583,9 @@
       <c r="D91" t="s">
         <v>786</v>
       </c>
+      <c r="E91">
+        <v>165600</v>
+      </c>
       <c r="F91" s="3" t="s">
         <v>823</v>
       </c>
@@ -9591,6 +9609,9 @@
       <c r="D92" t="s">
         <v>786</v>
       </c>
+      <c r="E92">
+        <v>81000</v>
+      </c>
       <c r="F92" s="3" t="s">
         <v>792</v>
       </c>
@@ -9613,6 +9634,9 @@
       </c>
       <c r="D93" t="s">
         <v>786</v>
+      </c>
+      <c r="E93">
+        <v>302000</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>793</v>

</xml_diff>

<commit_message>
just some simple work addons
</commit_message>
<xml_diff>
--- a/UploadedFiles/LocationData.xlsx
+++ b/UploadedFiles/LocationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DASHBOARDPROD1\c$\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dashboardProd1\c$\inetpub\wwwroot\MKCoop\UploadedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CCB16-B8AB-462A-B408-DC6CC10FCA80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E58B847-71BE-4D38-8E50-30670529B97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="872">
   <si>
     <t>Abilene</t>
   </si>
@@ -2640,6 +2640,9 @@
   </si>
   <si>
     <t>logo.png</t>
+  </si>
+  <si>
+    <t>HILLSBORO HOOP SHED</t>
   </si>
 </sst>
 </file>
@@ -2792,10 +2795,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M104" totalsRowShown="0">
-  <autoFilter ref="A1:M104" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M104">
-    <sortCondition ref="A2:A104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblTMALocations" displayName="tblTMALocations" ref="A1:M105" totalsRowShown="0">
+  <autoFilter ref="A1:M105" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M105">
+    <sortCondition ref="A2:A105"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="BRANCH_NUMBER"/>
@@ -3568,7 +3571,7 @@
   </sheetPr>
   <dimension ref="A1:AG70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7848,11 +7851,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9322,126 +9325,126 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B65" t="s">
-        <v>540</v>
+        <v>871</v>
       </c>
       <c r="D65" t="s">
         <v>647</v>
       </c>
-      <c r="E65">
-        <v>218560</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>536</v>
-      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B66" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="D66" t="s">
         <v>647</v>
       </c>
       <c r="E66">
-        <v>993000</v>
+        <v>218560</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B67" t="s">
-        <v>352</v>
+        <v>535</v>
       </c>
       <c r="D67" t="s">
         <v>647</v>
       </c>
       <c r="E67">
-        <v>550800</v>
+        <v>993000</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>9</v>
+        <v>534</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B68" t="s">
-        <v>527</v>
+        <v>352</v>
       </c>
       <c r="D68" t="s">
         <v>647</v>
       </c>
       <c r="E68">
-        <v>345600</v>
+        <v>550800</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>526</v>
+        <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="K68" s="3"/>
+        <v>530</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>432</v>
+        <v>361</v>
       </c>
       <c r="B69" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D69" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="E69">
-        <v>2255500</v>
-      </c>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+        <v>345600</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="K69" s="3"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B70" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D70" t="s">
         <v>645</v>
@@ -9449,792 +9452,809 @@
       <c r="E70">
         <v>2255500</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>520</v>
-      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="K70" s="3"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B71" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="D71" t="s">
         <v>645</v>
       </c>
       <c r="E71">
-        <v>867600</v>
+        <v>2255500</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B72" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="D72" t="s">
         <v>645</v>
       </c>
       <c r="E72">
-        <v>1293000</v>
+        <v>867600</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B73" t="s">
-        <v>641</v>
+        <v>514</v>
       </c>
       <c r="D73" t="s">
         <v>645</v>
       </c>
       <c r="E73">
-        <v>500000</v>
-      </c>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="K73" s="3"/>
+        <v>1293000</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B74" t="s">
-        <v>509</v>
+        <v>641</v>
       </c>
       <c r="D74" t="s">
         <v>645</v>
       </c>
       <c r="E74">
-        <v>900000</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>506</v>
-      </c>
+        <v>500000</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>510</v>
+        <v>447</v>
       </c>
       <c r="B75" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D75" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E75">
-        <v>1175000</v>
+        <v>900000</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="B76" t="s">
-        <v>354</v>
+        <v>505</v>
       </c>
       <c r="D76" t="s">
         <v>646</v>
       </c>
       <c r="E76">
-        <v>233100</v>
+        <v>1175000</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>109</v>
+        <v>504</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="B77" t="s">
-        <v>497</v>
+        <v>354</v>
       </c>
       <c r="D77" t="s">
         <v>646</v>
       </c>
       <c r="E77">
-        <v>326700</v>
+        <v>233100</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="B78" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="D78" t="s">
         <v>646</v>
       </c>
       <c r="E78">
-        <v>376200</v>
+        <v>326700</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B79" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="D79" t="s">
         <v>646</v>
       </c>
       <c r="E79">
-        <v>1053000</v>
+        <v>376200</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>484</v>
+        <v>489</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B80" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D80" t="s">
         <v>646</v>
       </c>
       <c r="E80">
-        <v>1040400</v>
+        <v>1053000</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B81" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="D81" t="s">
         <v>646</v>
       </c>
       <c r="E81">
-        <v>1356000</v>
+        <v>1040400</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B82" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="D82" t="s">
         <v>646</v>
       </c>
       <c r="E82">
-        <v>839000</v>
+        <v>1356000</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B83" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="D83" t="s">
         <v>646</v>
       </c>
       <c r="E83">
-        <v>529000</v>
+        <v>839000</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>465</v>
+        <v>470</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B84" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D84" t="s">
         <v>646</v>
       </c>
       <c r="E84">
-        <v>428000</v>
+        <v>529000</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B85" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="D85" t="s">
         <v>646</v>
       </c>
       <c r="E85">
-        <v>561000</v>
+        <v>428000</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B86" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="D86" t="s">
         <v>646</v>
       </c>
       <c r="E86">
-        <v>460000</v>
+        <v>561000</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B87" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="D87" t="s">
         <v>646</v>
       </c>
       <c r="E87">
-        <v>229000</v>
+        <v>460000</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>446</v>
+        <v>451</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B88" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D88" t="s">
         <v>646</v>
       </c>
       <c r="E88">
-        <v>312000</v>
+        <v>229000</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B89" t="s">
-        <v>396</v>
+        <v>445</v>
       </c>
       <c r="D89" t="s">
         <v>646</v>
       </c>
       <c r="E89">
-        <v>1400000</v>
+        <v>312000</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>181</v>
+        <v>444</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="B90" t="s">
-        <v>438</v>
+        <v>396</v>
       </c>
       <c r="D90" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E90">
-        <v>2800000</v>
-      </c>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="K90" s="3"/>
+        <v>1400000</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B91" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D91" t="s">
         <v>644</v>
       </c>
       <c r="E91">
-        <v>3600000</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>107</v>
-      </c>
+        <v>2800000</v>
+      </c>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="K91" s="3"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B92" t="s">
-        <v>823</v>
+        <v>437</v>
       </c>
       <c r="D92" t="s">
         <v>644</v>
       </c>
+      <c r="E92">
+        <v>3600000</v>
+      </c>
       <c r="F92" s="3" t="s">
-        <v>828</v>
+        <v>105</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>829</v>
-      </c>
-      <c r="H92" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="B93" t="s">
-        <v>436</v>
+        <v>823</v>
+      </c>
+      <c r="D93" t="s">
+        <v>644</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>435</v>
+        <v>828</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>433</v>
-      </c>
+        <v>829</v>
+      </c>
+      <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B94" t="s">
-        <v>643</v>
+        <v>436</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="H94" s="3"/>
+        <v>434</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>630</v>
+        <v>571</v>
       </c>
       <c r="B95" t="s">
-        <v>778</v>
-      </c>
-      <c r="D95" t="s">
-        <v>786</v>
+        <v>643</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>787</v>
+        <v>432</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>795</v>
-      </c>
-      <c r="H95" t="s">
-        <v>796</v>
-      </c>
-      <c r="K95" t="s">
-        <v>797</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B96" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D96" t="s">
         <v>786</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>798</v>
+        <v>795</v>
+      </c>
+      <c r="H96" t="s">
+        <v>796</v>
       </c>
       <c r="K96" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B97" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D97" t="s">
         <v>786</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>802</v>
+        <v>798</v>
+      </c>
+      <c r="K97" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B98" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D98" t="s">
         <v>786</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="K98" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B99" t="s">
-        <v>822</v>
+        <v>781</v>
       </c>
       <c r="D99" t="s">
         <v>786</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>824</v>
+        <v>790</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>825</v>
+        <v>803</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>826</v>
+        <v>804</v>
       </c>
       <c r="K99" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B100" t="s">
-        <v>782</v>
+        <v>822</v>
       </c>
       <c r="D100" t="s">
         <v>786</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>791</v>
+        <v>824</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>806</v>
+        <v>825</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
       <c r="K100" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B101" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D101" t="s">
         <v>786</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="K101" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B102" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D102" t="s">
         <v>786</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="K102" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B103" t="s">
-        <v>785</v>
+        <v>784</v>
+      </c>
+      <c r="D103" t="s">
+        <v>786</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="K103" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
+        <v>650</v>
+      </c>
+      <c r="B104" t="s">
+        <v>785</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="K104" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>940</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>642</v>
       </c>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>